<commit_message>
Fixed kit selection functionality
</commit_message>
<xml_diff>
--- a/miracuse_kits.xlsx
+++ b/miracuse_kits.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="192">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Attack</t>
   </si>
   <si>
-    <t xml:space="preserve">Venom applied to a weapon that turns flesh to stone, induces paralysis, or blinds the target. The user chooses which effect takes place.</t>
+    <t xml:space="preserve">Venom applied to a weapon that turns flesh to stone, induces paralysis, or causes significant pain. The user chooses which effect takes place.</t>
   </si>
   <si>
     <t xml:space="preserve">Beast’s Blood</t>
@@ -61,7 +61,16 @@
     <t xml:space="preserve">Utility</t>
   </si>
   <si>
-    <t xml:space="preserve">Potion that grants the user a dog’s sense of smell, a falcon’s sense of sight, or a bat’s sense of hearing. The user chooses which effect takes place.</t>
+    <t xml:space="preserve">Potion that grants the user a dog’s sense of smell, a falcon’s sense of sight, or a bat’s sense of hearing for a few hours. The user chooses which effect takes place.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dead Nettle Dust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, AoE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powder that does one of the following: induces uncontrollable sneezing, inflicts burns on exposed skin, or blinds. The user chooses which effect takes place. Can be applied to a weapon like a venom.</t>
   </si>
   <si>
     <t xml:space="preserve">Elixir</t>
@@ -73,55 +82,52 @@
     <t xml:space="preserve">Potion that recovers two Physical boxes or two Mental boxes. The user chooses which effect takes place.</t>
   </si>
   <si>
-    <t xml:space="preserve">Halcyon Vapor</t>
+    <t xml:space="preserve">Holy Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Attack, Defense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potion that renders the user inert to magic, making them highly resistant to spells, clearing away any lingering curses, and preventing them from using magic for a few hours. Can be applied to a weapon like a venom. Harmful to the undead and similar creatures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyde’s Draught</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Defense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potion that changes the user’s skin to one of the following: thin fireproof dragon scales, fish scales that let the user breathe underwater, or sticky scales that let the user climb with ease.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical Grenades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazard, AoE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that covers an area with a grease slick, a tangle of thick sticky webs, or a choking cloud of black smoke. The user chooses which effect takes place.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemental Grenades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, Hazard, AoE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that covers an area with searing flames, a sheet of ice, or crackling electricity. The user chooses which effect takes place.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flare Bullets</t>
   </si>
   <si>
     <t xml:space="preserve">Attack, Utility</t>
   </si>
   <si>
-    <t xml:space="preserve">Aerosol spray that induces vivid hallucinations. When used carefully, allows the user to see magic and spirits. When used offensively, induces paranoia and madness. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jekyll’s Draught</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Potion that allows the user to take Advantage on Physique or Agility rolls for the next few hours, but inflicts one Mental damage when consumed. The user chooses which effect takes place.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandman's Dust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Stealth, Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Powder that dazes and prevents new memories from being formed when breathed. When ingested, the user is compelled to speak truth and falls unconscious shortly after.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Munitions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical Grenades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hazard, AoE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with a grease slick, a tangle of sticky webs, or a thick cloud of smoke. The user chooses which effect takes place.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flare Bullets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bullet that burns hot and bright, piercing through stone, metal, and magic. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storm Grenades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Hazard, AoE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with searing flames, freezing ice, or crackling electricity. The user chooses which effect takes place.</t>
+    <t xml:space="preserve">Ammo that burns hot and bright, piercing through stone, metal, and magic. </t>
   </si>
   <si>
     <t xml:space="preserve">Timed Charge</t>
@@ -133,16 +139,16 @@
     <t xml:space="preserve">Trenchsteel Grenades</t>
   </si>
   <si>
+    <t xml:space="preserve">Attack, Utility, AoE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grenade that covers an area with hot metal caltrops, a bale of barbed wire, or flashing lights and deafening bangs. The user chooses which effect takes place.</t>
   </si>
   <si>
     <t xml:space="preserve">Trick Bullets</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Utility, AoE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elastic bullet that strikes with blunt force, knocking over targets and rebounding in closed spaces. Can change course mid-flight by detonating a second time.</t>
+    <t xml:space="preserve">Elastic ammo that strikes with blunt force, knocking over targets and rebounding in closed spaces. Can change course mid-flight by detonating a second time.</t>
   </si>
   <si>
     <t xml:space="preserve">Tools</t>
@@ -151,37 +157,37 @@
     <t xml:space="preserve">Bag of Holding</t>
   </si>
   <si>
-    <t xml:space="preserve">Bag that’s bigger on the inside than the outside. Items placed inside become weightless until withdrawn. </t>
+    <t xml:space="preserve">Bag that’s bigger on the inside than the outside. Items placed within become weightless until withdrawn. </t>
   </si>
   <si>
     <t xml:space="preserve">Boots of Traversing</t>
   </si>
   <si>
-    <t xml:space="preserve">A pair of boots that allow the wearer to walk on water, glide down when falling from great heights, and stick to walls.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clockwork Bird</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A mechanical bird that can fly, repeat spoken messages, stand watch, and carry out simple orders.</t>
+    <t xml:space="preserve">A pair of boots that allow the wearer to walk on water, glide down when falling from great heights, or stick to walls.</t>
   </si>
   <si>
     <t xml:space="preserve">Immovable Rod</t>
   </si>
   <si>
-    <t xml:space="preserve">Retractable pole that locks into place when activated, defying gravity and requiring immense force to move.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Philosopher’s Stone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gemstone that can transmute a substance into a similar substance when activated, such as changing metals into other metals. Effects fade over several hours.</t>
+    <t xml:space="preserve">Retractable steel pole that locks into place when activated, floating in defiance of gravity. Requires immense force to move. </t>
   </si>
   <si>
     <t xml:space="preserve">Quicksilver Homunculus</t>
   </si>
   <si>
-    <t xml:space="preserve">Sentient metal ooze that can change shape, becoming a platform, a weapon, or other object.</t>
+    <t xml:space="preserve">Sentient metal ooze that can change shape and hardness. Can be transformed into various tools, weapons, and objects when activated. Can follow simple orders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Transmutation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmute substances into other, similar substances. You can spend this Kit’s uses to apply Knowledge or Perception instead of Aura when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trumps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A deck of cards, each painted to resemble a person that the owner knows. When focusing on one or more cards, the user can communicate telepathically with the person on the card, provided that the target is willing and able.</t>
   </si>
   <si>
     <t xml:space="preserve">Mage</t>
@@ -310,7 +316,7 @@
     <t xml:space="preserve">Spirit of Sound</t>
   </si>
   <si>
-    <t xml:space="preserve">Amplify and quiet. Used to create and manipulate acoustics.</t>
+    <t xml:space="preserve">Amplify and quiet. Used to create and manipulate sound.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Thermos</t>
@@ -322,127 +328,103 @@
     <t xml:space="preserve">Scoundrel</t>
   </si>
   <si>
-    <t xml:space="preserve">Scout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use Cunning or Agility when scouting an area. You can use a Prep Point to learn an enemy’s weakness or find an alternative entrance to a location.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beastmaster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have Advantage on all rolls against animals and monsters. You can spend a Prep Point to mesmerize animals and monsters, preventing them from acting for a short time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camouflage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stealth, Attack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“Assume a Disguise” can be used to assume the appearance of an object or of terrain. You can use a Prep Point to make a ranged sneak attack without breaking your disguise.</t>
+    <t xml:space="preserve">Ranger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beast Tamer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You enlist a local animal to assist you. The animal can track, warn you of danger, fight, and do anything a creature of its kind might. You can speak with and understand the animal. You can compel the animal to do something it doesn’t want to by spending a Prep Point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lifesense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can sense the presence or absence of life nearby. You can spend a Prep Point to extend your range by a significant amount, or to sense the general emotional state of any creature in range.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piper’s Flute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have a musical instrument that attracts and influences nearby creatures when played. You can spend a Prep Point to do one of the following: mesmerize an animal or animal-like creature, lull unwary creatures to sleep, or incite them to rampage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Prep Points. When you use a Prep Point to change Kits, you can change two Kits instead of one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of plant matter. You can spend a Prep Point to use Cunning or Agility instead of Aura when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning or Agility when scouting areas, tracking a target, or collecting information. You can spend a Prep Point to know an enemy’s weakness, find a secret entrance to a location, or find a lead in an investigation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assassinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sneak attacks inflict an additional point of damage. You can spend a Prep Point to enter stealth, even from combat or while in plain sight.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social, Prep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characters met through “I Know a Guy” owe you a favor, and tend to be highly placed in organizations. You can spend a Prep Point to declare that you have blackmail against a target provided that you could reasonably justify having prepared blackmail ahead of time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contingency Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Health, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The items from “What You Needed” can be less plausible and more valuable, reflecting your ability to plan for all eventualities. You can spend a Prep Point to recover a Mental box and vice versa. Can be done once per action if used in combat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convincing Fake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose a Skill you have no points in, and treat it as half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate.</t>
   </si>
   <si>
     <t xml:space="preserve">Infiltration Team</t>
   </si>
   <si>
+    <t xml:space="preserve">Stealth, Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. “Assume a Disguise” also produces disguises for your allies. You can use a Prep Point to prevent you or your allies from being revealed when they otherwise would be.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iocane Powder</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stealth</t>
   </si>
   <si>
-    <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. You can use a Prep Point to prevent you or your allies from being revealed when they otherwise would be.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prepared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional two Prep Points. When you use a Prep Point to change Kits, you can change two Kits instead of one.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trapper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can spend a Prep Point to do one of the following without breaking stealth: restrain a target, inflict Physical damage to a target, or sound an alarm if a target crosses a threshold.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assassinate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sneak attacks inflict an additional point of damage. You can spend a Prep Point to enter stealth, even from combat or while in plain sight.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social, Prep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Characters met through “I Know a Guy” owe you a favor, and tend to be highly placed in organizations. You can spend a Prep Point to declare that you have blackmail against a target provided that you could reasonably justify having prepared blackmail ahead of time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contingency Plan</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Spend a Mental box to recover a Prep Point or vice versa. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Can be done once per action if performed in combat.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Convincing Fake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose a Skill you have no points in, and treat it as half the level of your highest Skill (rounded down). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entourage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stealth, Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“Assume a Disguise” also provides disguises for all of your allies. They use your Cunning for the purposes of the disguise.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thespian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning as though it were Aura, Bravery, or Knowledge for social purposes. You can spend a Prep Point to credibly impersonate a Mage, Soldier, or Alchemist while doing so, as though you had used “Assume a Disguise”.</t>
+    <t xml:space="preserve">You can put unwary targets to sleep with a pinch of this alchemic poison. You can expend a Prep Point to use a higher concentration version, which will additionally wipe away the target’s memory of the day. Unsuitable for use in combat.</t>
   </si>
   <si>
     <t xml:space="preserve">Swashbuckler</t>
@@ -454,7 +436,7 @@
     <t xml:space="preserve">Defense</t>
   </si>
   <si>
-    <t xml:space="preserve">When you successfully defend against a Physical attack you can do one of the following: inflict Physical damage on the attacker, redirect the attack to a nearby enemy, or disarm the attacker. You can spend a Prep Point to succeed at defending regardless of your roll.</t>
+    <t xml:space="preserve">When you successfully defend against a Physical attack you can also choose to do one of the following: inflict Physical damage on the attacker, redirect the attack to a nearby enemy, or disarm the attacker. You can spend a Prep Point to succeed at defending regardless of your roll.</t>
   </si>
   <si>
     <t xml:space="preserve">Arta Forteiza</t>
@@ -466,199 +448,157 @@
     <t xml:space="preserve">Gain an additional Physical box. You can spend a Prep Point to recover one Physical box. Requires an action when performed in combat.</t>
   </si>
   <si>
+    <t xml:space="preserve">Arta Loquit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning as though it were Aura, Bravery, or Knowledge for social purposes. When you do so you can “Adopt a Disguise” to assume an alias without spending a Prep Point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arta Siva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning to provoke and intimidate in combat. When you succeed on provoking or intimidating an enemy in combat, you recover a Prep Point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arta Tuco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you make an attack you can also choose to do one of the following: move, use an item, or grant Advantage to the next person attacking that enemy. You can spend a Prep Point to inflict a sneak attack regardless of stealth.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arta Valar</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">When you make an attack you can do one of the following: target Mental health rather than Physical, steal something from your target, or delay the target’s next turn in combat. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">You can spend a Prep Point to take an action in combat when it isn’t your turn. </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Bravo</t>
+    <t xml:space="preserve">When you make an attack you can also choose to do one of the following in addition to dealing damage: target Mental health rather than Physical, steal something from your target, or delay the target’s next turn in combat. You can spend a Prep Point to take an action in combat when it isn’t your turn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discipline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Boundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, Defense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take a free attack against enemies that attempt to enter or leave your melee range. You can spend a Fortune Point to prevent enemies and attacks from moving past you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Guard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can defend against Physical attacks with Physique or Bravery. You can spend a Fortune Point to protect a nearby ally from harm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your rally recovers a Physical or Mental box for the target when used in combat. User chooses which effect takes place. You can spend a Fortune Point to revive an incapacitated ally using rally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Sights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks, both melee and ranged, have a longer range than normal. You can spend a Fortune Point to make a nearly impossible shot with pinpoint accuracy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Vigil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Physique or Bravery when watching for danger or sensing motives. You can spend a Fortune Point at the beginning of combat to take one action before anyone else.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Will</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional Mental box. You can spend a Fortune Point to recover a Mental box and vice versa. Can be done once per action if used in combat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gambler’s Fallacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You recover a Fortune Point when you roll a 1. You can spend a Fortune Point to guarantee a 10 on your next action without rolling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jackpot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you roll a 10 you take a +3 instead of a +2 to the result. You can spend a Fortune Point to increase your roll number by 1 (i.e. a 1 would become a 2, a 2 would become a 3, and so on). The roll number cannot increase beyond 10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Fortune Point boxes. When you use a Fortune Point to reroll, add a +1 to the reroll result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near Miss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you roll a 1 you take a +0 instead of a -2 to the result. You can spend a Fortune Point to avoid taking damage from an attack or hazard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Chance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bend probability in your favor or against others. You can spend a Fortune Point to use Physique or Bravery instead of Aura when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winning Charm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You make a good first impression, acquiring the respect or affection of people you meet. You can spend a Fortune Point to establish a reputation of your choice among those you meet for the first time, regardless of whether or not it’s deserved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hordebreaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When make an attack, you can also choose to damage a second enemy. You can spend a Fortune Point to damage all enemies in combat or hit several targets simultaneously outside of combat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mindbreaker</t>
   </si>
   <si>
     <t xml:space="preserve">Attack, Social</t>
   </si>
   <si>
-    <t xml:space="preserve">You can provoke and intimidate using Cunning. Enemies that you provoke/intimidate take Mental damage. You can use a Prep Point to provoke or intimidate all enemies in combat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Honor Among Thieves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Teamwork regardless of whether or not you have the Skill required to assist. You can use a Prep Point to give an ally your action in combat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subtlety</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you make an attack you can do one of the following: move, use an item, or grant Advantage to the next person attacking that enemy. You can spend a Prep Point to inflict a sneak attack regardless of stealth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soldier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discipline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bulletproof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use Physique or Bravery when defending against Physical attacks. You can spend a Fortune Point to make a melee counterattack on a successful defense.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hold the Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your rally recovers a Physical or Mental box for the target when used in combat. You can spend a Fortune Point to revive an incapacitated ally using rally.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Will</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health, Defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional Mental box. You can spend a Fortune Point to avoid taking Mental damage from attacks and hazards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make Your Own Luck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spend a Mental box to recover a Fortune Point or vice versa. Can be done once per action if performed in combat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Watchful and Ready</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use Physique or Bravery when watching for danger or sensing motives. You can spend a Fortune Point at the beginning of combat to take one action before anyone else.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone of Control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take a free attack against enemies that attempt to enter or leave your melee range. You can spend a Fortune Point to protect a nearby ally from harm.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fortune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balanced Karma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you roll a 1, recover a Fortune Point. You can spend a Fortune Point to guarantee a 10 on your next roll.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bringer of Misfortune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enemies that harm you are jinxed. The next attack against them has Advantage. You can spend a Fortune Point when provoking or intimidating to proclaim a curse, gaining Advantage on all rolls against the target for a few hours.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fortune’s Favorite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When rolling a 1, you take a +0 instead of a -2. You can spend a Fortune Point to avoid taking damage from an attack.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lucky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional two Fortune Point boxes. When you use a Fortune Point to reroll, add a +1 to the reroll result.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manipulate Probability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chance bends in your favor whenever something would otherwise be left up to luck. You can spend a Fortune Point to nudge probability more strongly, though never quite beyond the bounds of reason.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Winning Charm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You make a good first impression, acquiring the respect or affection of people you meet. You can spend a Fortune Point to establish a reputation of your choice among a crowd, regardless of whether or not it’s deserved.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blitz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you attack you can also do one of the following: attack a second target near the first, provoke/intimidate an enemy, or rally an ally. You can spend a Fortune Point to attack all enemies in combat. Use one roll to determine attack outcomes for multiple attacks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Break the Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks also do one of the following: force an enemy to move, knock an enemy over, or prevent an enemy from moving. You can spend a Fortune Point to send an appropriately-sized enemy or object flying through the air.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Called Shot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks also do one of the following: damage an enemy’s equipment, target a specific part of anatomy, or hit from a longer range than normal. You can spend a Fortune Point to attempt to destroy an object outright.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deadly Grace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use Physique or Bravery for the purposes of movement and determining turn order. You can spend a Fortune Point to make two attacks in one action.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heroic Determination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you would otherwise be incapacitated, mark the relevant injury instead. Cannot be used when the injury is already marked. You can spend a Fortune Point to ignore the negative effects of an injury until your next rest.</t>
+    <t xml:space="preserve">When you provoke or intimidate a sentient enemy, they take Mental damage. You can spend a Fortune Point to demoralize someone you’ve provoked or intimidated, gaining Advantage on all rolls against them while they’re affected.</t>
   </si>
   <si>
     <t xml:space="preserve">Spellbreaker</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Take Advantage on all rolls to defend against magic. Your attacks can damage spells and spirits. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">You can spend a Fortune Point to deflect a spell back at its caster or clear away magical effects in the area.</t>
-    </r>
+    <t xml:space="preserve">Take Advantage on all rolls to defend against magic. Your attacks can damage spells and spirits. You can spend a Fortune Point to deflect a spell back at its caster or clear away magical effects in the area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stancebreaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you make an attack, you can also choose to knock your target over, pin them in place, or force them to reposition, in addition to dealing damage. You can spend a Fortune Point to make an attack that launches an appropriately-sized enemy or object into the air.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swordbreaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you make an attack, you can also choose to damage your target’s equipment or a specific part of their anatomy, in addition to dealing damage. You can spend a Fortune Point to make an attack that outright destroys an object or obstacle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willbreaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you make an attack, you can also choose to provoke or intimidate an enemy, in addition to dealing damage. You can spend a Fortune Point to provoke or intimidate all enemies in combat at the same time.</t>
   </si>
 </sst>
 </file>
@@ -669,7 +609,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -729,19 +669,6 @@
       <name val="Fira Sans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Fira Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Fira Sans"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -868,7 +795,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -926,10 +853,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1077,11 +1000,11 @@
   </sheetPr>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
@@ -1186,10 +1109,10 @@
         <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1200,13 +1123,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1214,16 +1137,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1231,16 +1154,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1248,16 +1171,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1265,16 +1188,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1282,16 +1205,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1299,16 +1222,16 @@
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1316,16 +1239,16 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1333,16 +1256,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1350,16 +1273,16 @@
         <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1367,16 +1290,16 @@
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1384,16 +1307,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1401,353 +1324,353 @@
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>105</v>
@@ -1755,169 +1678,169 @@
     </row>
     <row r="40" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>106</v>
       </c>
       <c r="D40" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C41" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="E41" s="14" t="s">
         <v>110</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C42" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="E44" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C45" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C46" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C47" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="E47" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C48" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="E48" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C49" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>133</v>
@@ -1925,7 +1848,7 @@
     </row>
     <row r="50" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>134</v>
@@ -1942,12 +1865,12 @@
     </row>
     <row r="51" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="13" t="s">
         <v>138</v>
       </c>
       <c r="D51" s="13" t="s">
@@ -1959,7 +1882,7 @@
     </row>
     <row r="52" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>134</v>
@@ -1968,7 +1891,7 @@
         <v>141</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>142</v>
@@ -1976,7 +1899,7 @@
     </row>
     <row r="53" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>134</v>
@@ -1993,7 +1916,7 @@
     </row>
     <row r="54" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>134</v>
@@ -2002,7 +1925,7 @@
         <v>146</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>147</v>
@@ -2010,7 +1933,7 @@
     </row>
     <row r="55" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>134</v>
@@ -2026,309 +1949,309 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="C56" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="D56" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="E56" s="19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="16" t="s">
+      <c r="E57" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B58" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C57" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="16" t="s">
+      <c r="C58" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B59" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C58" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="16" t="s">
+      <c r="C59" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B60" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C59" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="16" t="s">
+      <c r="C60" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B61" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C60" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="16" t="s">
+      <c r="C61" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B61" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="E61" s="19" t="s">
+      <c r="B62" s="16" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="16" t="s">
+      <c r="C62" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B62" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D62" s="18" t="s">
+      <c r="B63" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="D63" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="18" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16" t="s">
+    <row r="64" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B63" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C63" s="18" t="s">
+      <c r="B64" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D63" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="19" t="s">
+      <c r="D64" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E64" s="18" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="16" t="s">
+    <row r="65" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B64" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C64" s="18" t="s">
+      <c r="B65" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C65" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D65" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E65" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="E64" s="19" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="17" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="16" t="s">
+      <c r="D66" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B65" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E65" s="19" t="s">
+      <c r="B67" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" s="17" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="16" t="s">
+      <c r="D67" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E67" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B66" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E66" s="19" t="s">
+      <c r="B68" s="16" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="16" t="s">
+      <c r="C68" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B67" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="16" t="s">
+      <c r="B69" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B68" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="D68" s="18" t="s">
+      <c r="B70" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="16" t="s">
+      <c r="E71" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B69" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="D69" s="18" t="s">
+      <c r="B72" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D73" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E69" s="19" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C71" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="E72" s="19" t="s">
+      <c r="E73" s="18" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E73" s="19" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to gameplay kits
</commit_message>
<xml_diff>
--- a/miracuse_kits.xlsx
+++ b/miracuse_kits.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="202">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -80,6 +80,318 @@
   </si>
   <si>
     <t xml:space="preserve">Halcyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When used as a potion, allows the user to see, speak with, and touch spirits. When used as a venom, induces violent hallucinations and Mental damage. Considered a worthy offering by many magical creatures. Can be thrown as a grenade to inflict Mental damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, Defense, Utility, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When used as a potion, clears away curses and renders the user highly resistant to magic. When used as a venom, prevents targets from using magic for a few hours. Harmful to the undead and corrosive to magic. Can be thrown as a grenade to purge magical effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golemcraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bronze Homunculus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A set of bronze knives with blades on both ends of its hilt. When activated, it will seek out its owner’s enemies (or a nearby target of their choice) and attack as though it has a mind of its own. Only one knife can be thrown in an action, but multiple knives can be active at once.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloth Homunculus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A cloak that resists gravity, allowing the wearer to glide when falling. When activated, can be used as a flying carpet for a short period of time, or as a bag that renders objects inside weightless.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper Homunculus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A deck of cards painted to resemble people that the Alchemist knows. When focusing on one or more cards, the user can communicate telepathically with the person on the card, provided that the target is willing and able. You can spend a use to create a card of yourself that can be given to others. A card created this way will last seven days before crumbling to dust.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quicksilver Homunculus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Defense, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A liquid metal bracer that can change shape on command, becoming a variety of tools or melee weapons. You can spend a use to have the bracer protect you from a Physical attack, such as an arrow or sword swing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Transmutation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Magic, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform substances into other, similar substances. You can spend this Kit’s uses to apply Knowledge or Perception instead of Aura when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steel Homunculus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A steel staff that can change size and weight on command, from pocket-sized to 10 feet long, and from a few pounds to a few hundred pounds. You can spend a use to lock the staff in place, strongly resisting any force that tries to move it and floating in defiance of gravity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chemical Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazard, AoE, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that covers an area with a grease slick, quick drying cement, or a choking cloud of black smoke. Can be used as a bullet to produce a smaller but more precise effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnesium Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, AoE, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that creates blinding light or a deafening whistle. When used as a bullet, can penetrate cover and deals additional Physical damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storm Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, Hazard, AoE, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that covers an area with crackling electricity or magnetizes an area, forcing metal objects in the vicinity to adhere to one another. Can be used as a bullet to produce a smaller but more precise effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermal Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that covers an area with searing flames or a sheet of ice. Can be used as a bullet to produce a smaller but more precise effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tranquilizer Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, AoE, Stealth, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that covers an area in a fog of sleeping powder, knocking the unwary unconscious and dazing others. Can be used as a bullet to produce a smaller but more precise effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trenchsteel Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that creates a swarm of bouncing metal ball bearings or a bale of barbed wire. When used as a bullet, can change course mid-flight by detonating a second time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celestial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Divination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seek and learn. Used to scry for hidden things and reveal new information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Heavens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, Utility, Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smite and cleanse. Used to punish evil and dispel magic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Hells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrupt and wrong. Used to raise the dead and subvert the natural order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social, Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speak and understand. Used to communicate with all manner of creatures, including animals and monsters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Restoration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recovery, Utility, Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore and repair. Used to heal wounds and mend broken objects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Warding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defense, Utility, Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seal and repel. Used to create barriers and push targets away.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Aether</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of electricity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of air.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of earth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Flame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of flame.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of water.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemental </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of magnetism.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fundamental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Binding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adhere and restrain. Used to lash things together with gravitational force.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Entropy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dissolve and decay. Used to unravel targets into their base elements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Social, Stealth, Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brighten and dim. Used to create and manipulate illusory images.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Locomotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accelerate and slow. Used to manipulate kinetic energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amplify and quiet. Used to create and manipulate sound.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Thermos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat and cool. Used to manipulate thermal energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scoundrel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beast Tamer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, Utility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You enlist a local animal to assist you. The animal can track, warn you of danger, fight, and do anything a creature of its kind might. You can speak with and understand the animal. You can compel the animal to do something it doesn’t want to by spending a Prep Point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lifesense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can sense the presence or absence of life nearby. You can spend a Prep Point to extend your range by a significant amount, or to sense the emotions of any creature in range. You have Advantage when sensing the motives of another person.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piper’s Flute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have a musical instrument that attracts and influences nearby creatures when played. You can spend a Prep Point to do one of the following: mesmerize an animal or monster, lull unwary creatures to sleep, or incite them to rampage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Prep Points. When you use a Prep Point to change Kits, you can change two Kits instead of one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of plant matter. You can spend a Prep Point to use Cunning or Agility instead of Aura when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning or Agility when scouting areas, tracking a target, or collecting information. You can spend a Prep Point to learn an enemy’s weakness, find a secret entrance to a location, or find a clue in an investigation. You take Advantage against traps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assassinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack, Stealth</t>
   </si>
   <si>
     <r>
@@ -90,7 +402,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">When used as a potion, allows the user to see, speak with, and touch spirits. When used as a venom, induces violent hallucinations and Mental damage. Considered a worthy offering by many magical creatures. </t>
+      <t xml:space="preserve">Your sneak attacks deal additional damage, and do not break stealth when the target is incapacitated. </t>
     </r>
     <r>
       <rPr>
@@ -99,14 +411,23 @@
         <rFont val="Fira Sans"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Can be thrown as a grenade to inflict Mental damage.</t>
+      <t xml:space="preserve">You can spend a Prep Point to enter stealth, even from combat or while in plain sight.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Holy Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Defense, Utility, Alchemy</t>
+    <t xml:space="preserve">Convincing Fake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose a Skill you have no points in, and treat it as half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infiltration Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stealth, Social</t>
   </si>
   <si>
     <r>
@@ -117,7 +438,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">When used as a potion, clears away curses and renders the user highly resistant to magic. When used as a venom, prevents targets from using magic for a few hours. Harmful to the undead and corrosive to magic. </t>
+      <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. </t>
     </r>
     <r>
       <rPr>
@@ -126,346 +447,7 @@
         <rFont val="Fira Sans"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Can be thrown as a grenade to purge magical effects.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Golemcraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bronze Homunculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A set of bronze knives with blades on both ends of its hilt. When activated, it will seek out its owner’s enemies (or a nearby target of their choice) and attack as though it has a mind of its own. Only one knife can be thrown in an action, but multiple knives can be active at once.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cloth Homunculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A cloak that resists gravity, allowing the wearer to glide when falling. When activated, can be used as a flying carpet for a short period of time, or as a bag that renders objects inside weightless.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paper Homunculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A deck of cards painted to resemble people that the Alchemist knows. When focusing on one or more cards, the user can communicate telepathically with the person on the card, provided that the target is willing and able. You can spend a use to create a card of yourself that can be given to others. A card created this way will last seven days before crumbling to dust.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quicksilver Homunculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Defense, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A liquid metal bracer that can change shape on command, becoming a variety of tools or melee weapons. You can spend a use to have the bracer protect you from a Physical attack, such as an arrow or sword swing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Transmutation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Magic, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transform substances into other, similar substances. You can spend this Kit’s uses to apply Knowledge or Perception instead of Aura when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steel Homunculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A steel staff that can change size and weight on command, from pocket-sized to 10 feet long, and from a few pounds to a few hundred pounds. You can spend a use to lock the staff in place, strongly resisting any force that tries to move it and floating in defiance of gravity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Munitions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chemical Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hazard, AoE, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with a grease slick, quick drying cement, or a choking cloud of black smoke. Can be used as a bullet to produce a smaller but more precise effect.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnesium Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, AoE, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that creates blinding light or a deafening whistle. When used as a bullet, can penetrate cover and deals additional Physical damage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storm Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Hazard, AoE, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with crackling electricity or magnetizes an area, forcing metal objects in the vicinity to adhere to one another. Can be used as a bullet to produce a smaller but more precise effect.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermal Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with searing flames or a sheet of ice. Can be used as a bullet to produce a smaller but more precise effect.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tranquilizer Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, AoE, Stealth, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area in a fog of Iocane powder, knocking the unwary unconscious and dazing others. Can be used as a bullet to produce a smaller but more precise effect.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trenchsteel Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that creates a swarm of bouncing metal ball bearings or a bale of barbed wire. When used as a bullet, can change course mid-flight by detonating a second time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Celestial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Divination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seek and learn. Used to scry for hidden things and reveal new information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Heavens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Utility, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smite and cleanse. Used to punish evil and dispel magic.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Hells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corrupt and wrong. Used to raise the dead and subvert the natural order.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speak and understand. Used to communicate with all manner of creatures, including animals and monsters.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Restoration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recovery, Utility, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore and repair. Used to heal wounds and mend broken objects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Warding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defense, Utility, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seal and repel. Used to create barriers and push targets away.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elemental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Aether</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of electricity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of air.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Earth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of earth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Flame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of flame.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of water.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elemental </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Force</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of magnetism.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fundamental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Binding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adhere and restrain. Used to lash things together with gravitational force.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Entropy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolve and decay. Used to unravel targets into their base elements.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Social, Stealth, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brighten and dim. Used to create and manipulate illusory images.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Locomotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accelerate and slow. Used to manipulate kinetic energy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Sound</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amplify and quiet. Used to create and manipulate sound.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Thermos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heat and cool. Used to manipulate thermal energy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoundrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beast Tamer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Utility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You enlist a local animal to assist you. The animal can track, warn you of danger, fight, and do anything a creature of its kind might. You can speak with and understand the animal. You can compel the animal to do something it doesn’t want to by spending a Prep Point.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lifesense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can sense the presence or absence of life nearby. You can spend a Prep Point to extend your range by a significant amount, or to sense the emotions of any creature in range. You have Advantage when sensing the motives of another person.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piper’s Flute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have a musical instrument that attracts and influences nearby creatures when played. You can spend a Prep Point to do one of the following: mesmerize an animal or monster, lull unwary creatures to sleep, or incite them to rampage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prepared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional two Prep Points. When you use a Prep Point to change Kits, you can change two Kits instead of one.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of plant matter. You can spend a Prep Point to use Cunning or Agility instead of Aura when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning or Agility when scouting areas, tracking a target, or collecting information. You can spend a Prep Point to learn an enemy’s weakness, find a secret entrance to a location, or find a clue in an investigation. You take Advantage against traps.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assassinate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sneak attacks inflict an additional point of damage. You can spend a Prep Point to enter stealth, even from combat or while in plain sight. When your sneak attack incapacitates a target, you do not break stealth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social, Prep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Characters met through “I Know a Guy” owe you a favor, and tend to be highly placed in organizations. You can spend a Prep Point to declare that you have blackmail against a target provided that you could reasonably justify having prepared blackmail ahead of time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contingency Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Health, Recovery</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">The items from “What You Needed” can be less plausible and more valuable, reflecting your ability to plan for all eventualities. You can convert a Prep Point to a Mental box or vice versa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, and can do so once per action while in combat.</t>
+      <t xml:space="preserve">“Assume a Disguise” also produces disguises for your allies. </t>
     </r>
     <r>
       <rPr>
@@ -475,53 +457,32 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">You can use a Prep Point to prevent you or your allies from being revealed when they otherwise would be. </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Convincing Fake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose a Skill you have no points in, and treat it as half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infiltration Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stealth, Social</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. You can use a Prep Point to prevent you or your allies from being revealed when they otherwise would be. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">“Assume a Disguise” also produces disguises for your allies.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Iocane Powder</t>
   </si>
   <si>
     <t xml:space="preserve">Stealth</t>
   </si>
   <si>
-    <t xml:space="preserve">You can put unwary targets to sleep with a pinch of an alchemic poison. You can expend a Prep Point to use a higher concentration version, which will additionally wipe away the target’s memory of the day. Unsuitable for use in combat.</t>
+    <t xml:space="preserve">Your sneak attacks can put targets to sleep and wipe away their memory instead of incapacitating them. You can spend a Prep Point to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadowdancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can move your shadow independently of your body. Your shadow can interact with physical objects, including moving objects and attacking enemies. You can spend a Prep Point to teleport from one shadowed area to another within sight. You can see perfectly in the dark.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spycraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility, Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Assume a Disguise” is nearly instantaneous, and includes an alias. “What You Needed” can produce forgeries of documents and symbols of authority. “I Know a Guy” can be used to produce blackmail on targets.</t>
   </si>
   <si>
     <t xml:space="preserve">Swashbuckler</t>
@@ -542,25 +503,7 @@
     <t xml:space="preserve">Health, Recovery</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Gain an additional Physical box. You can convert a Prep Point into Physical box or vice versa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, and can do so once per action while in combat. </t>
-    </r>
+    <t xml:space="preserve">Gain an additional Physical box. You can convert a Prep Point into Physical box or vice versa, and can do so once per action while in combat. </t>
   </si>
   <si>
     <t xml:space="preserve">Arta Loquit</t>
@@ -608,25 +551,7 @@
     <t xml:space="preserve">Iron Blood</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">You are immune to most environmental hazards, including magical and alchemical hazards. You can spend a Fortune Point to weaponize an environmental hazard, such as sweeping a weapon through an open flame and sending flames at your enemies. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Poisons and similar afflictions have no effect on you. </t>
-    </r>
+    <t xml:space="preserve">You are immune to most environmental hazards, including magical and alchemical hazards. You can spend a Fortune Point to weaponize an environmental hazard, such as sweeping a weapon through an open flame and sending flames at your enemies. Poisons and similar afflictions have no effect on you. </t>
   </si>
   <si>
     <t xml:space="preserve">Iron Circle</t>
@@ -1158,10 +1083,10 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E48" activeCellId="0" sqref="E48"/>
+      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
@@ -1980,10 +1905,10 @@
         <v>133</v>
       </c>
       <c r="D48" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E48" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1994,13 +1919,13 @@
         <v>120</v>
       </c>
       <c r="C49" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="E49" s="14" t="s">
         <v>137</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2008,16 +1933,16 @@
         <v>103</v>
       </c>
       <c r="B50" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="D50" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="E50" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2025,16 +1950,16 @@
         <v>103</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C51" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="E51" s="14" t="s">
         <v>144</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2042,16 +1967,16 @@
         <v>103</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C52" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="E52" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2059,16 +1984,16 @@
         <v>103</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C53" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="E53" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2076,16 +2001,16 @@
         <v>103</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C54" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="E54" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2093,322 +2018,322 @@
         <v>103</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C55" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="E55" s="14" t="s">
         <v>156</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B56" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="C56" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="D56" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="18" t="s">
         <v>160</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B57" s="16" t="s">
-        <v>159</v>
-      </c>
       <c r="C57" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" s="18" t="s">
         <v>162</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B58" s="16" t="s">
-        <v>159</v>
-      </c>
       <c r="C58" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E58" s="18" t="s">
         <v>164</v>
-      </c>
-      <c r="D58" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B59" s="16" t="s">
-        <v>159</v>
-      </c>
       <c r="C59" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="E59" s="18" t="s">
         <v>167</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B60" s="16" t="s">
-        <v>159</v>
-      </c>
       <c r="C60" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D60" s="17" t="s">
         <v>106</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B61" s="16" t="s">
-        <v>159</v>
-      </c>
       <c r="C61" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" s="18" t="s">
         <v>171</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B62" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C62" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="D62" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="E62" s="18" t="s">
         <v>175</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C63" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D63" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="E63" s="18" t="s">
         <v>178</v>
-      </c>
-      <c r="E63" s="18" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D64" s="17" t="s">
         <v>114</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C65" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E65" s="18" t="s">
         <v>182</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="E65" s="18" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D66" s="17" t="s">
         <v>59</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C67" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="18" t="s">
         <v>186</v>
-      </c>
-      <c r="D67" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B68" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C68" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="D68" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="E68" s="18" t="s">
         <v>190</v>
-      </c>
-      <c r="E68" s="18" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C69" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E69" s="18" t="s">
         <v>192</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="E69" s="18" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C70" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D70" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="D70" s="17" t="s">
+      <c r="E70" s="18" t="s">
         <v>195</v>
-      </c>
-      <c r="E70" s="18" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C71" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E71" s="18" t="s">
         <v>197</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="E71" s="18" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>106</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C73" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E73" s="18" t="s">
         <v>201</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E73" s="18" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More minor kit changes
</commit_message>
<xml_diff>
--- a/miracuse_kits.xlsx
+++ b/miracuse_kits.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="193">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Basilisk Tongue</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Utility, Alchemy</t>
+    <t xml:space="preserve">Exploration, Alchemy</t>
   </si>
   <si>
     <t xml:space="preserve">When used as a potion, gives the user stone-like skin for a few hours. When used as a venom, turns flesh to stone. Can be applied to stone to make it soft as clay for a few hours. Can be thrown as a grenade to turn stone to mud.</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Dead Nettle Dust</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Utility, AoE, Alchemy</t>
+    <t xml:space="preserve">Combat, Recovery, Alchemy</t>
   </si>
   <si>
     <t xml:space="preserve">When used as a potion, numbs the user to pain and mitigates the effects of Injuries. When used as a venom, causes severe pain and additional Physical damage. Induces violent coughing when breathed. Can be thrown as a grenade to inflict Physical damage.</t>
@@ -82,15 +82,15 @@
     <t xml:space="preserve">Halcyon</t>
   </si>
   <si>
+    <t xml:space="preserve">Combat, Exploration, Alchemy</t>
+  </si>
+  <si>
     <t xml:space="preserve">When used as a potion, allows the user to see, speak with, and touch spirits. When used as a venom, induces violent hallucinations and Mental damage. Considered a worthy offering by many magical creatures. Can be thrown as a grenade to inflict Mental damage.</t>
   </si>
   <si>
     <t xml:space="preserve">Holy Water</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Defense, Utility, Alchemy</t>
-  </si>
-  <si>
     <t xml:space="preserve">When used as a potion, clears away curses and renders the user highly resistant to magic. When used as a venom, prevents targets from using magic for a few hours. Harmful to the undead and corrosive to magic. Can be thrown as a grenade to purge magical effects.</t>
   </si>
   <si>
@@ -100,37 +100,37 @@
     <t xml:space="preserve">Bronze Homunculus</t>
   </si>
   <si>
+    <t xml:space="preserve">Combat, Alchemy</t>
+  </si>
+  <si>
     <t xml:space="preserve">A set of bronze knives with blades on both ends of its hilt. When activated, it will seek out its owner’s enemies (or a nearby target of their choice) and attack as though it has a mind of its own. Only one knife can be thrown in an action, but multiple knives can be active at once.</t>
   </si>
   <si>
     <t xml:space="preserve">Cloth Homunculus</t>
   </si>
   <si>
-    <t xml:space="preserve">Utility, Alchemy</t>
-  </si>
-  <si>
     <t xml:space="preserve">A cloak that resists gravity, allowing the wearer to glide when falling and run across water. When activated, can be used as a flying carpet for a short period of time, or as a bag that renders objects inside weightless.</t>
   </si>
   <si>
     <t xml:space="preserve">Paper Homunculus</t>
   </si>
   <si>
+    <t xml:space="preserve">Exploration, Social, Alchemy</t>
+  </si>
+  <si>
     <t xml:space="preserve">A deck of cards painted to resemble people that the Alchemist knows. When focusing on one or more cards, the user can communicate telepathically with the person on the card, provided that the target is willing and able. You can spend a use to create a card of yourself that can be given to others. A card created this way will last seven days before crumbling to dust.</t>
   </si>
   <si>
     <t xml:space="preserve">Quicksilver Homunculus</t>
   </si>
   <si>
-    <t xml:space="preserve">Utility, Defense, Alchemy</t>
-  </si>
-  <si>
     <t xml:space="preserve">A liquid metal bracer that can change shape on command, becoming a variety of tools or melee weapons. You can spend a use to have the bracer shield you from a Physical attack by expanding into a large metal disc.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Transmutation</t>
   </si>
   <si>
-    <t xml:space="preserve">Utility, Magic, Alchemy</t>
+    <t xml:space="preserve">Magic, Alchemy</t>
   </si>
   <si>
     <t xml:space="preserve">Transform substances into other, similar substances. You can spend this Kit’s uses to apply Knowledge or Perception instead of Aura when using this spirit.</t>
@@ -148,27 +148,18 @@
     <t xml:space="preserve">Chemical Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Hazard, AoE, Alchemy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grenade that covers an area with a grease slick, quick drying cement, or a choking cloud of black smoke. Can be used as a bullet to produce a smaller but more precise effect.</t>
   </si>
   <si>
     <t xml:space="preserve">Magnesium Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, AoE, Alchemy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grenade that creates blinding light or a deafening whistle. When used as a bullet, can penetrate cover and deals additional Physical damage.</t>
   </si>
   <si>
     <t xml:space="preserve">Storm Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Hazard, AoE, Alchemy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grenade that covers an area with crackling electricity or magnetizes an area, forcing metal objects in the vicinity to adhere to one another. Can be used as a bullet to produce a smaller but more precise effect.</t>
   </si>
   <si>
@@ -181,9 +172,6 @@
     <t xml:space="preserve">Tranquilizer Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, AoE, Stealth, Alchemy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grenade that covers an area in a fog of sleeping powder, knocking the unwary unconscious and dazing others. Can be used as a bullet to produce a smaller but more precise effect.</t>
   </si>
   <si>
@@ -202,7 +190,7 @@
     <t xml:space="preserve">Spirit of Divination</t>
   </si>
   <si>
-    <t xml:space="preserve">Utility, Magic</t>
+    <t xml:space="preserve">Exploration, Magic</t>
   </si>
   <si>
     <t xml:space="preserve">Seek and learn. Used to scry for hidden things and reveal new information.</t>
@@ -211,7 +199,7 @@
     <t xml:space="preserve">Spirit of Heavens</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Utility, Magic</t>
+    <t xml:space="preserve">Combat, Magic</t>
   </si>
   <si>
     <t xml:space="preserve">Smite and cleanse. Used to punish evil and dispel magic.</t>
@@ -220,6 +208,9 @@
     <t xml:space="preserve">Spirit of Hells</t>
   </si>
   <si>
+    <t xml:space="preserve">Magic</t>
+  </si>
+  <si>
     <t xml:space="preserve">Corrupt and wrong. Used to raise the dead and subvert the natural order.</t>
   </si>
   <si>
@@ -235,7 +226,7 @@
     <t xml:space="preserve">Spirit of Restoration</t>
   </si>
   <si>
-    <t xml:space="preserve">Recovery, Utility, Magic</t>
+    <t xml:space="preserve">Recovery, Magic</t>
   </si>
   <si>
     <t xml:space="preserve">Restore and repair. Used to heal wounds and mend broken objects.</t>
@@ -244,9 +235,6 @@
     <t xml:space="preserve">Spirit of Warding</t>
   </si>
   <si>
-    <t xml:space="preserve">Defense, Utility, Magic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Seal and repel. Used to create barriers and push targets away.</t>
   </si>
   <si>
@@ -256,6 +244,9 @@
     <t xml:space="preserve">Spirit of Aether</t>
   </si>
   <si>
+    <t xml:space="preserve">Combat, Exploration, Magic</t>
+  </si>
+  <si>
     <t xml:space="preserve">Allows for control and limited manifestation of electricity.</t>
   </si>
   <si>
@@ -310,9 +301,6 @@
     <t xml:space="preserve">Spirit of Light</t>
   </si>
   <si>
-    <t xml:space="preserve">Utility, Social, Stealth, Magic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Brighten and dim. Used to create and manipulate illusory images.</t>
   </si>
   <si>
@@ -343,7 +331,7 @@
     <t xml:space="preserve">Beast Tamer</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Utility</t>
+    <t xml:space="preserve">Combat, Exploration</t>
   </si>
   <si>
     <t xml:space="preserve">You enlist a local animal to assist you. The animal can track, warn you of danger, fight, and do anything a creature of its kind might. You can speak with and understand the animal. You can compel the animal to do something it doesn’t want to by spending a Prep Point.</t>
@@ -352,16 +340,16 @@
     <t xml:space="preserve">Lifesense</t>
   </si>
   <si>
-    <t xml:space="preserve">Utility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can sense the presence or absence of life nearby. You can spend a Prep Point to extend your range by a significant amount, or to sense the emotions of any creature in range. You have Advantage when sensing the motives of another person.</t>
+    <t xml:space="preserve">Exploration, Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can sense the presence or absence of life nearby. You can spend a Prep Point to extend your range by a significant amount for a short time, or to read the emotions of any creature in range. You have Advantage when sensing the motives of another person.</t>
   </si>
   <si>
     <t xml:space="preserve">Piper’s Flute</t>
   </si>
   <si>
-    <t xml:space="preserve">You have a musical instrument that attracts the attention of nearby creatures when played. You can spend a Prep Point to do one of the following: calm an animal or animal-like monster, or incite them to rampage. You have Advantage on all rolls against related creatures.</t>
+    <t xml:space="preserve">You have a musical instrument that attracts the attention of nearby animal-like creatures and spirits when played. You can spend a Prep Point to either calm them or stir them into a frenzy. You have Advantage on all rolls against related creatures.</t>
   </si>
   <si>
     <t xml:space="preserve">Prepared</t>
@@ -379,10 +367,13 @@
     <t xml:space="preserve">Allows for control and limited manifestation of plant matter. You can spend a Prep Point to use Cunning or Agility instead of Aura when using this spirit.</t>
   </si>
   <si>
-    <t xml:space="preserve">Tracker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning or Agility when scouting areas, tracking a target, or collecting information. You can spend a Prep Point to learn an enemy’s weakness, find a secret entrance to a location, or find a clue in an investigation. You take Advantage against traps.</t>
+    <t xml:space="preserve">Tracker’s Trade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social, Exploration, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning or Agility when actively collecting information, and can disguise yourself as terrain via “Assume a Disguise” without expending a Prep Point. You can spend a Prep Point to learn an enemy’s weakness, uncover a secret entrance to a location, or find a clue in an investigation. You take Advantage against traps.</t>
   </si>
   <si>
     <t xml:space="preserve">Spy</t>
@@ -391,97 +382,22 @@
     <t xml:space="preserve">Assassinate</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your sneak attacks deal additional damage, and do not break stealth when the target is incapacitated. You can spend a Prep Point to enter stealth, even from combat or while in plain sight. Doing so takes an action in combat.</t>
+    <t xml:space="preserve">Combat, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your sneak attacks deal additional damage. You can spend a Prep Point to enter stealth, even from combat or while in plain sight. Doing so takes an action in combat. Sneak attacks that incapacitate an enemy do not break stealth.</t>
   </si>
   <si>
     <t xml:space="preserve">Convincing Fake</t>
   </si>
   <si>
-    <t xml:space="preserve">Utility, Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose a Skill you have no points in, and treat it as half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate.</t>
+    <t xml:space="preserve">Choose a Skill you have no points in, and raise it to half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate.</t>
   </si>
   <si>
     <t xml:space="preserve">Infiltration Team</t>
   </si>
   <si>
-    <t xml:space="preserve">Stealth, Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. “Assume a Disguise” also produces disguises for your allies. You can use a Prep Point to prevent you or your allies from being revealed when they otherwise would be. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iocane Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stealth, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your sneak attacks can put targets to sleep and wipe away their memory instead of incapacitating them. Successfully doing so recovers a Prep Point.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shadowdancing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can move your shadow independently of your body. Your shadow can interact with physical objects, including moving objects and attacking enemies, but takes your action to do so. You can spend a Prep Point to switch places with your shadow. You can see perfectly in the dark.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spycraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“Assume a Disguise” is nearly instantaneous, and allows you to adopt an alias with a legally documented background and history. “What You Needed” can produce forgeries of documents, symbols of authority, and similar items. “I Know a Guy” can be used to produce blackmail on targets.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swashbuckler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Eres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can counterattack or move after successfully defending against an attack. You can spend a Prep Point to succeed at defending against an attack regardless of your roll. You can move before and after taking an action in combat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Forteiza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional Physical box. You can convert a Prep Point into Physical box or vice versa, and can do so once per action while in combat. You do not need to sleep, and cannot be rendered unconscious, though you may be incapacitated through other means.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Loquit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning as though it were Aura, Bravery, or Knowledge for social purposes. When you do so you can “Adopt a Disguise” without spending a Prep Point. You can spend a Prep Point to reroll any social action you take, up to one additional time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Siva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning or Agility to provoke and intimidate in combat. When you succeed on provoking or intimidating an enemy in combat, you recover a Prep Point.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Tuco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack, Defense</t>
+    <t xml:space="preserve">Social, Stealth</t>
   </si>
   <si>
     <r>
@@ -492,7 +408,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">You can steal from a target on a successful attack or defense. You can spend a Prep Point to inflict a sneak attack regardless of stealth. </t>
+      <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. You can use a Prep Point to prevent you or your allies from being revealed when they otherwise would be. </t>
     </r>
     <r>
       <rPr>
@@ -501,16 +417,76 @@
         <rFont val="Fira Sans"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Using a single item as an action does not end your turn in combat, though subsequent uses will.</t>
+      <t xml:space="preserve">“Assume a Disguise” also produces disguises for your allies.</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Iocane Powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Stealth, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your sneak attacks can put targets to sleep and wipe away their short-term memory instead of incapacitating them. Successfully doing so recovers a Prep Point. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadowdancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can move your shadow independently of your body. Your shadow can interact with physical objects, including moving objects and attacking enemies, but takes your action to do so. You can spend a Prep Point to switch places with your shadow. You can see perfectly in the dark.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spycraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Assume a Disguise” is nearly instantaneous, and allows you to adopt an alias with a legally documented background and history. “What You Needed” can produce forgeries of documents, symbols of authority, and similar items. “I Know a Guy” can be used to produce blackmail on targets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swashbuckler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arta Eres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can counterattack or move after successfully defending against an attack. You can spend a Prep Point to succeed at defending against an attack regardless of your roll. You can move before and after taking an action in combat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arta Forteiza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional Physical box. You can convert a Prep Point into Physical box or vice versa, and can do so once per action while in combat. You do not need to sleep, and cannot be rendered unconscious, though you may be incapacitated through other means.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arta Loquit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning as though it were Aura, Bravery, or Knowledge for social purposes. When you do so you can “Adopt a Disguise” without spending a Prep Point. You can spend a Prep Point to reroll any social action you take, up to one additional time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arta Siva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning or Agility to provoke and intimidate in combat. When you succeed on provoking or intimidating an enemy in combat, you recover a Prep Point.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arta Tuco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can steal from a target on a successful attack or defense. You can spend a Prep Point to inflict a sneak attack regardless of stealth. Using a single item as an action does not end your turn in combat, though subsequent uses will.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arta Valar</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack</t>
-  </si>
-  <si>
     <t xml:space="preserve">Your attacks can target Mental health instead of Physical. You can spend a Prep Point to take an action before someone else, including taking actions outside of your turn in combat. You can use this ability a maximum of one time between your normal turns in combat. You always go first when turn order is declared. </t>
   </si>
   <si>
@@ -523,13 +499,16 @@
     <t xml:space="preserve">Iron Blood</t>
   </si>
   <si>
-    <t xml:space="preserve">You are immune to most environmental hazards, including magical and alchemical hazards. You can spend a Fortune Point to weaponize an environmental hazard, such as sweeping a weapon through an open flame and sending flames at your enemies. Poisons and similar afflictions have no effect on you. </t>
+    <t xml:space="preserve">Exploration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are immune to most environmental hazards, including magical and alchemical hazards. You can spend a Fortune Point to weaponize an environmental hazard, such as sweeping a weapon through an open flame and sending fire at your enemies. Poisons and similar afflictions have no effect on you. </t>
   </si>
   <si>
     <t xml:space="preserve">Iron Circle</t>
   </si>
   <si>
-    <t xml:space="preserve">Take a free attack against enemies that attempt to enter or leave your melee range. You can spend a Fortune Point to prevent enemies and attacks from moving past you. You are immune to sneak attacks and take Advantage against traps.</t>
+    <t xml:space="preserve">Take a free attack against enemies that attempt to enter or leave your melee range. You can spend a Fortune Point to prevent enemies and attacks from moving past you. You are immune to sneak attacks and similar effects.</t>
   </si>
   <si>
     <t xml:space="preserve">Iron Stance</t>
@@ -541,10 +520,10 @@
     <t xml:space="preserve">Iron Star</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks also count as a rally for one ally. You can spend a Fortune Point to revive an incapacitated ally using a rally. When you recover Physical or Mental health, you recover one more box than you would otherwise.</t>
+    <t xml:space="preserve">Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks rally an ally, requiring no additional rolls when successful. You can spend a Fortune Point to revive an incapacitated ally using a rally. When you recover Physical or Mental health, you recover one more box than you would otherwise.</t>
   </si>
   <si>
     <t xml:space="preserve">Iron Strength</t>
@@ -565,18 +544,15 @@
     <t xml:space="preserve">Curse</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Those you provoke or intimidate are prone to bouts of misfortune. You can spend a Fortune Point to make such a curse into a lasting weakness. For example, cursing someone to suffer more from blades, fire, or heartbreak.</t>
+    <t xml:space="preserve">Combat, Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Those you provoke or intimidate are prone to bouts of misfortune. The next roll against them, from you or your allies, has Advantage. You can spend a Fortune Point to change this effect into a lasting weakness affiliated with a specific threat (fire, blades, poverty, etc.) Rolls related to this threat have Advantage against the target.</t>
   </si>
   <si>
     <t xml:space="preserve">Gambler’s Fallacy</t>
   </si>
   <si>
-    <t xml:space="preserve">Recovery</t>
-  </si>
-  <si>
     <t xml:space="preserve">You recover a Fortune Point when you roll a 1. You can spend a Fortune Point to guarantee a 10 on your next action without rolling.</t>
   </si>
   <si>
@@ -601,7 +577,10 @@
     <t xml:space="preserve">Winning Charm</t>
   </si>
   <si>
-    <t xml:space="preserve">You make a good first impression, acquiring the respect or affection of people you meet. You can spend a Fortune Point to establish a reputation of your choice among those you meet for the first time, regardless of whether or not it’s deserved.</t>
+    <t xml:space="preserve">Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You make a good first impression, acquiring the respect or affection of people you meet. You can spend a Fortune Point to establish a reputation of your choice among those you meet for the first time, regardless of whether or not it’s deserved. You have Advantage when using Bravery or Physique to impress others.</t>
   </si>
   <si>
     <t xml:space="preserve">Valor</t>
@@ -610,43 +589,37 @@
     <t xml:space="preserve">Hordebreaker</t>
   </si>
   <si>
-    <t xml:space="preserve">Attack, AoE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks affect anyone or anything near your target. You can spend a Fortune Point to make an attack against every enemy in combat, or to strike one target twice.</t>
+    <t xml:space="preserve">Your attacks affect anyone or anything near your target, becoming area-of-effect. You can spend a Fortune Point to make an attack against every enemy in combat, or to strike one target twice. Take Advantage when attacking groups of enemies.</t>
   </si>
   <si>
     <t xml:space="preserve">Skybreaker</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks, both melee and ranged, have a much longer range than normal. You can spend a Fortune Point to make a nearly impossible shot with pinpoint accuracy.</t>
+    <t xml:space="preserve">Your attacks, both melee and ranged, have a much longer range than normal. You can spend a Fortune Point to make a nearly impossible shot with pinpoint accuracy. When you tie attacking an enemy, you succeed instead of the defender.</t>
   </si>
   <si>
     <t xml:space="preserve">Spellbreaker</t>
   </si>
   <si>
-    <t xml:space="preserve">Utility, Attack, Defense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks can damage spells and spirits. You can spend a Fortune Point to deflect a spell back at its caster or clear away magical effects in the area.</t>
+    <t xml:space="preserve">Your attacks can damage spells and spirits. You can spend a Fortune Point to deflect a spell back at its caster or clear away magical effects in the area. Take Advantage when attacking mages or spirits.</t>
   </si>
   <si>
     <t xml:space="preserve">Stancebreaker</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks push targets back. You can spend a Fortune Point to forcefully reposition a target; knocking it down, pinning it in place, launching it into the air, or throwing it a great distance.</t>
+    <t xml:space="preserve">Your attacks force enemies to reposition and volley objects into the air. You can spend a Fortune Point to manipulate a target’s placement; knocking it down, pinning it in place, launching it into the air, or throwing it a great distance. Enemies that you hit have reduced movement throughout combat.</t>
   </si>
   <si>
     <t xml:space="preserve">Swordbreaker</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks can strike through stone and metal, damaging equipment and piercing cover as well as causing harm. You can spend a Fortune Point to outright destroy an object or obstacle.</t>
+    <t xml:space="preserve">Your attacks can strike through stone and metal, damaging equipment and piercing cover as well as causing harm. You can spend a Fortune Point to outright destroy an object or obstacle. Take Advantage when attacking armored enemies.</t>
   </si>
   <si>
     <t xml:space="preserve">Willbreaker</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks also count as provoking or intimidating. You can spend a Fortune Point to exploit the weakness of anyone you’ve provoked or intimidated, taking Advantage on all rolls against them while they’re still influenced.</t>
+    <t xml:space="preserve">Your attacks provoke or intimidate, requiring no additional rolls to produce either effect when successful. You can spend a Fortune Point to succeed in getting your target’s full attention. Take Advantage when attacking enemies influenced by your provocation or intimidation.</t>
   </si>
 </sst>
 </file>
@@ -1054,11 +1027,11 @@
   </sheetPr>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
@@ -1163,10 +1136,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1177,10 +1150,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>22</v>
@@ -1197,10 +1170,10 @@
         <v>24</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1211,10 +1184,10 @@
         <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>28</v>
@@ -1231,10 +1204,10 @@
         <v>29</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1245,10 +1218,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>33</v>
@@ -1282,7 +1255,7 @@
         <v>37</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>38</v>
@@ -1299,10 +1272,10 @@
         <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1313,13 +1286,13 @@
         <v>39</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1330,13 +1303,13 @@
         <v>39</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1347,13 +1320,13 @@
         <v>39</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1364,13 +1337,13 @@
         <v>39</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1381,931 +1354,931 @@
         <v>39</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="D21" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="D27" s="9" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>92</v>
-      </c>
       <c r="D33" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B39" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="13" t="s">
-        <v>108</v>
-      </c>
       <c r="D39" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>120</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B51" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="D51" s="13" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>152</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" s="18" t="s">
         <v>157</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="D58" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B59" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="C59" s="17" t="s">
-        <v>165</v>
-      </c>
       <c r="D59" s="17" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B64" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E64" s="18" t="s">
         <v>172</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="E64" s="18" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>194</v>
+        <v>136</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B71" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C71" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C71" s="17" t="s">
-        <v>196</v>
-      </c>
       <c r="D71" s="17" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Patch before a larger refactor
</commit_message>
<xml_diff>
--- a/miracuse_kits.xlsx
+++ b/miracuse_kits.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="197">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -43,31 +43,16 @@
     <t xml:space="preserve">Alchemist</t>
   </si>
   <si>
-    <t xml:space="preserve">Drugs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basilisk Tongue</t>
+    <t xml:space="preserve">Chemist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beast’s Blood</t>
   </si>
   <si>
     <t xml:space="preserve">Exploration, Alchemy</t>
   </si>
   <si>
-    <t xml:space="preserve">When used as a potion, gives the user stone-like skin for a few hours. When used as a venom, turns flesh to stone. Can be applied to stone to make it soft as clay for a few hours. Can be thrown as a grenade to turn stone to mud.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beast’s Blood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When used as a potion, grants the user an enhanced sense (sight, hearing, or smell) for several hours. When used as a venom, steals away senses (sight, hearing, or smell). Can be used to attract animals and monsters. Can be thrown as a grenade to bait animals and monsters.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dead Nettle Dust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Recovery, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When used as a potion, numbs the user to pain and mitigates the effects of Injuries. When used as a venom, causes severe pain and additional Physical damage. Induces violent coughing when breathed. Can be thrown as a grenade to inflict Physical damage.</t>
+    <t xml:space="preserve">Adopt an animal-like adaption for a short period of time by drinking a potion. Example of effects could include a cat’s night vision, a bat’s sense of hearing, or a gecko’s skin.</t>
   </si>
   <si>
     <t xml:space="preserve">Elixir</t>
@@ -76,37 +61,49 @@
     <t xml:space="preserve">Recovery, Alchemy</t>
   </si>
   <si>
-    <t xml:space="preserve">When used as a potion, recovers two Physical boxes or two Mental boxes. When used as a venom, inflicts cursed wounds that resist healing. Cleanses poisons, diseases, and rot. Not usable as a grenade.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Halcyon</t>
+    <t xml:space="preserve">Recover from harm and illness by drinking a potion. This can include recovering two boxes of Physical damage, recovering two boxes of Mental damage, treating an Injury, or curing various natural afflictions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faerie Fire</t>
   </si>
   <si>
     <t xml:space="preserve">Combat, Exploration, Alchemy</t>
   </si>
   <si>
-    <t xml:space="preserve">When used as a potion, allows the user to see, speak with, and touch spirits. When used as a venom, induces violent hallucinations and Mental damage. Considered a worthy offering by many magical creatures. Can be thrown as a grenade to inflict Mental damage.</t>
+    <t xml:space="preserve">Cause burning pain and violent coughing by throwing a highly volatile dust. Capable of creating dazzling fireworks displays, conducting electricity, and producing abundant colorful smoke when exposed to fire. Can be used as a grenade to inflict Physical damage.</t>
   </si>
   <si>
     <t xml:space="preserve">Holy Water</t>
   </si>
   <si>
-    <t xml:space="preserve">When used as a potion, clears away curses and renders the user highly resistant to magic. When used as a venom, prevents targets from using magic for a few hours. Harmful to the undead and corrosive to magic. Can be thrown as a grenade to purge magical effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golemcraft</t>
+    <t xml:space="preserve">Neutralize magic by spraying specially treated water. Can be used to negate spells, ward away monsters, create light, or produce anti-magic effects. Can be used as a grenade to dampen magical effects over a wide area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manifold Venom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cause additional harm and effects by applying poisons to weapon. These might include additional Physical damage, temporary blindness, or gradual petrification.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaper’s Oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reshape stone and metal by rubbing an ointment into them. Possible applications might include creating a shelter in rock, opening an entry to a brick building, or bending metal bars. Can be used as a grenade to turn areas of solid dirt or rock into quicksand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enchanter</t>
   </si>
   <si>
     <t xml:space="preserve">Clay Homunculus</t>
   </si>
   <si>
-    <t xml:space="preserve">A set of polished quartz stones. Planting one in dirt or mud creates a small clay golem, roughly three feet tall. The golem will follow its creator’s orders for one hour or until it is destroyed, whichever comes first. It has little intelligence and is able to fight.</t>
+    <t xml:space="preserve">Create a clay golem from mud or dirt. The golem is roughly three feet tall, will follow your orders, and is capable of fighting on your behalf. It will fall apart one hour after its creation.</t>
   </si>
   <si>
     <t xml:space="preserve">Cloth Homunculus</t>
   </si>
   <si>
-    <t xml:space="preserve">A cloak that resists gravity, allowing the wearer to glide when falling and run across water. When activated, can be used as a flying carpet for a short period of time, or as a bag that renders objects inside weightless.</t>
+    <t xml:space="preserve">Create a cloak out of living cloth. The cloak lightens the weight of its user, allowing them to fall from great distances without harm. On command the cloak can also become 200 ft. of sturdy rope, a bag that reduces the weight of its contents, or another object made of thread. The cloak remains active so long as this Kit is equipped.</t>
   </si>
   <si>
     <t xml:space="preserve">Paper Homunculus</t>
@@ -115,31 +112,31 @@
     <t xml:space="preserve">Exploration, Social, Alchemy</t>
   </si>
   <si>
-    <t xml:space="preserve">A deck of cards painted to resemble people that the Alchemist knows. When focusing on one or more cards, the user can communicate telepathically with the person on the card, provided that the target is willing and able. You can spend a use to create a card of yourself that can be given to others. A card created this way will last seven days before crumbling to dust.</t>
+    <t xml:space="preserve">Create a shikigami, a flying talisman made of paper. The talisman can carry messages, eavesdrop, and scout. It has Cunning equal to half your Knowledge rounded down. The talisman will fall apart one hour after its creation.</t>
   </si>
   <si>
     <t xml:space="preserve">Quicksilver Homunculus</t>
   </si>
   <si>
-    <t xml:space="preserve">A liquid metal bracer that can change shape on command, becoming a variety of tools or melee weapons. You can spend a use to have the bracer shield you from a Physical attack by expanding into a large metal disc.</t>
+    <t xml:space="preserve">Create a shapeshifting metal familiar, generally worn as a bracelet when not in use. Without expending any of this Kit’s uses, the familiar can change into simple metal objects like tools and weapons. The creator can expend a use to perform more complex or fast-paced transformations. Examples might include a shield to deflect an incoming attack, a musical instrument, or a bear trap. The familiar remains active so long as this Kit is equipped.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awaken and imbue with purpose. Used to compel objects to move with a life of their own. You can spend this Kit’s uses to use Knowledge or Perception when using this spirit.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Transmutation</t>
   </si>
   <si>
-    <t xml:space="preserve">Magic, Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transform substances into other, similar substances. You can spend this Kit’s uses to apply Knowledge or Perception instead of Aura when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steel Homunculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A steel staff that can change size and weight on command, from pocket-sized to 10 feet long, and from a featherweight to a few hundred pounds. You can spend a use to lock the staff in place, strongly resisting any force that tries to move it and floating in defiance of gravity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Munitions</t>
+    <t xml:space="preserve">Transform and alter. Used to change the properties of a substance, such as shape and weight. The greater the difference from the original, the more difficult the change. You can spend this Kit’s uses to use Knowledge or Perception when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sapper</t>
   </si>
   <si>
     <t xml:space="preserve">Concussive Charges</t>
@@ -148,25 +145,25 @@
     <t xml:space="preserve">Combat, Alchemy</t>
   </si>
   <si>
-    <t xml:space="preserve">Grenade that ruptures the ground or stuns those in area with bright light and deafening sound. When used as a bullet, can penetrate cover and deal additional Physical damage.</t>
+    <t xml:space="preserve">Grenade that ruptures the ground or stuns those in the area with bright light and deafening sound. When used as a bullet, successful attacks deal an additional box of Physical damage.</t>
   </si>
   <si>
     <t xml:space="preserve">Electromagnetic Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Grenade that covers an area with crackling electricity or magnetizes an area, forcing metal objects in the vicinity to adhere to one another. Can be used as a bullet to produce a smaller but more precise effect.</t>
+    <t xml:space="preserve">Grenade that covers an area with crackling electricity or magnetizes an area, forcing metal objects in the vicinity to adhere to one another. Can be used as a bullet to produce a smaller but more potent effect.</t>
   </si>
   <si>
     <t xml:space="preserve">Friction Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Grenade that covers an area with a grease slick or quick-drying adhesive. Can be used as a bullet to produce a smaller but more precise effect.</t>
+    <t xml:space="preserve">Grenade that covers an area with a grease slick or quick-drying adhesive. Can be used as a bullet to produce a smaller but more potent effect.</t>
   </si>
   <si>
     <t xml:space="preserve">Thermic Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Grenade that covers an area with roaring flames or a layer of ice. Can be used as a bullet to produce a smaller but more precise effect.</t>
+    <t xml:space="preserve">Grenade that covers an area with roaring flames or a layer of ice. Can be used as a bullet to produce a smaller but more potent effect.</t>
   </si>
   <si>
     <t xml:space="preserve">Trenchsteel Charges</t>
@@ -178,13 +175,22 @@
     <t xml:space="preserve">Vapor Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Grenade that covers an area in scalding steam or a billowing cloud of fog. When used as a bullet, can instantly rust metals.</t>
+    <t xml:space="preserve">Grenade that covers an area in scalding steam or a billowing cloud of fog. When used as a bullet, can instantly rust through metals.</t>
   </si>
   <si>
     <t xml:space="preserve">Mage</t>
   </si>
   <si>
-    <t xml:space="preserve">Celestial</t>
+    <t xml:space="preserve">Priest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Abjuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seal and purify. Used to create barriers and dispel magic.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Divination</t>
@@ -196,31 +202,22 @@
     <t xml:space="preserve">Seek and learn. Used to scry for hidden things and reveal new information.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Heavens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smite and cleanse. Used to punish evil and dispel magic.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Hells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corrupt and wrong. Used to raise the dead and subvert the natural order.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spirit of Language</t>
   </si>
   <si>
     <t xml:space="preserve">Social, Magic</t>
   </si>
   <si>
-    <t xml:space="preserve">Speak and understand. Used to communicate with all manner of creatures, including animals and monsters.</t>
+    <t xml:space="preserve">Speak and understand. Used to commune with all creatures and compel others to your will.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Necromancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Magic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrupt and wrong. Used to raise the dead and curse the living.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Restoration</t>
@@ -232,21 +229,18 @@
     <t xml:space="preserve">Restore and repair. Used to heal wounds and mend broken objects.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Warding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seal and repel. Used to create barriers and push targets away.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elemental</t>
+    <t xml:space="preserve">Spirit of Summoning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petition and conjure. Used to pull otherworldly influences into the mortal realm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaman</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Aether</t>
   </si>
   <si>
-    <t xml:space="preserve">Combat, Exploration, Magic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Allows for control and limited manifestation of electricity.</t>
   </si>
   <si>
@@ -268,85 +262,178 @@
     <t xml:space="preserve">Allows for control and limited manifestation of flame.</t>
   </si>
   <si>
+    <t xml:space="preserve">Spirit of Metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows for control and limited manifestation of metal.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spirit of Water</t>
   </si>
   <si>
     <t xml:space="preserve">Allows for control and limited manifestation of water.</t>
   </si>
   <si>
-    <t xml:space="preserve">Elemental </t>
+    <t xml:space="preserve">Wizard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Binding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adhere and restrain. Used to lash things together with gravitational force.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Entropy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diminish and dissolve. Used to unravel targets into their base elements.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Force</t>
   </si>
   <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of magnetism.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fundamental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Binding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adhere and restrain. Used to lash things together with gravitational force.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Entropy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolve and decay. Used to unravel targets into their base elements.</t>
+    <t xml:space="preserve">Channel raw magical energy. Used to lob bolts of force at enemies, or otherwise manipulate resevoirs of energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Locomotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accelerate and slow. Used to manipulate kinetic energy, adding or taking away speed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Reinforcement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortify and empower. Used to improve existing qualities, such as making someone stronger or faster.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Thermos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat and cool. Used to manipulate thermal energy, adding or taking away temperature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scoundrel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assassin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assassinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your sneak attacks deal an additional box of Physical damage. You can use "Assume a Disguise" to disappear from sight, even in the middle of combat. You can tell if a target will be incapacitated by your sneak attack before you make it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convincing Fake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration, Social, Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose a Skill you have no points in, and raise it to half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate. You can use “Assume a Disguise” without spending Prep Points.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infiltration Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. When you use "Assume a Disguise", you can provide disguises to your allies as well. When you or an ally would otherwise be revealed, you can spend a Prep Point to prevent it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iocane Powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Social, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your sneak attacks can put targets to sleep and cause short-term memory loss. You can use "What You Needed" to produce a vial of liquid that makes those who drink it highly suggestible. Those under the effects of the liquid will speak truthfully, but are visibly drugged, and slow to react.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Shadow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obscure and muffle. Used to manipulate darkness and quiet footsteps. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unbounded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locks, magic barriers, illusions, and similar obstacles fall apart at your touch. You can use "What You Needed" to produce specialized tools for infiltration, such as forged documents or badges of office. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charm Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning as though it were Aura, Bravery, or Knowledge for social purposes. You can spend a Prep Point to reroll a social action and take the new result, a maximum of one time per social action. You can use "I Know a Guy" without spending Prep Points.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning or Agility to detect and identify magic. You can use "What You Needed" to produce an item that briefly channels or negates magic you've identified. You can use Cunning or Agility when recalling information about history, religion, magic, or politics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resilience Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health, Exploration, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional Physical box. You can exchange Mental boxes for Prep Points and vice versa, and can do so as an action while in combat. You do not need to sleep, and cannot be rendered unconscious against your will, but can be incapacitated in other ways.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Light</t>
   </si>
   <si>
-    <t xml:space="preserve">Brighten and dim. Used to create and manipulate illusory images.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Locomotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accelerate and slow. Used to manipulate kinetic energy.</t>
+    <t xml:space="preserve">Brighten and bend light. Used to create and manipulate illusory images, as well as to see afar. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Sound</t>
   </si>
   <si>
-    <t xml:space="preserve">Combat, Social, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amplify and quiet. Used to create and manipulate sound.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Thermos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heat and cool. Used to manipulate thermal energy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoundrel</t>
+    <t xml:space="preserve">Amplify and distort. Used to create and manipulate sound, as well as to listen in from a distance. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">War Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique allows you to move before and after making an attack. You can spend a Prep Point to take an additional action on your turn, besides another attack. You can expend a Prep Point to combine this technique with another.</t>
   </si>
   <si>
     <t xml:space="preserve">Ranger</t>
   </si>
   <si>
-    <t xml:space="preserve">Beast Tamer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration, Social, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can communicate with animals, and use “I Know a Guy” to enlist a local animal to assist you. The animal can track, warn you of danger, fight, and do anything a creature of its kind might. You can compel the animal to do something it doesn’t want to by spending a Prep Point. You recover a Prep Point when you defeat an animal or animal-like monster.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hunter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social, Exploration, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning or Agility when actively collecting information, and can disguise yourself as terrain via “Assume a Disguise”. You can spend a Prep Point to uncover a secret entrance, find another exit, or find a clue in an investigation. You have Advantage against traps.</t>
+    <t xml:space="preserve">Camouflage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your sneak attacks do not reveal your position or break stealth, though they may alert enemies to your presence. You can use "Assume a Disguise" to take on the appearance of terrain or common objects, such as trees or crates.</t>
   </si>
   <si>
     <t xml:space="preserve">Lifesense</t>
@@ -355,13 +442,13 @@
     <t xml:space="preserve">Exploration, Social</t>
   </si>
   <si>
-    <t xml:space="preserve">You can use Cunning or Agility when interacting with spirits, and can sense the presence or absence of life nearby. You can spend a Prep Point to greatly extend your range, or to sense the emotions of those in range. You have Advantage when sensing motives and know when others lie.</t>
+    <t xml:space="preserve">You can sense the presence and absence of life using Cunning or Agility. You can use "I Know a Guy" to focus your senses, feeling the emotions of those nearby and knowing when they tell lies. When performing magic of any kind you can use Cunning or Agility as the primary Skill, and do not need to expend a Prep Point to do so.</t>
   </si>
   <si>
     <t xml:space="preserve">Prepared</t>
   </si>
   <si>
-    <t xml:space="preserve">Health</t>
+    <t xml:space="preserve">Exploration, Health</t>
   </si>
   <si>
     <t xml:space="preserve">Gain an additional two Prep Points. When you use a Prep Point to change Kits, you can change two Kits instead of one. You can use “What You Needed” without spending Prep Points.</t>
@@ -373,244 +460,160 @@
     <t xml:space="preserve">Combat, Recovery</t>
   </si>
   <si>
-    <t xml:space="preserve">You can use “What You Needed” to produce a weapon or ammunition that target a specific enemy’s weakness, provided that you know what the weakness is. Attacks made with the item deal additional damage. You can spend a Prep Point to discover an enemy’s weakness. You recover a Prep Point anytime you or your allies defeat an enemy with its weakness.</t>
+    <t xml:space="preserve">You instinctively know the weaknesses of monsters and beasts. You can use "What You Needed" to produce a weapon or ammunition that's particularly effective against them. Attacks with this item inflict an additional box of Physical damage. When you or an ally incapacitate an enemy with its weakness, you recover a Prep Point.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Wood</t>
   </si>
   <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of plant matter. You can spend a Prep Point to use Cunning or Agility instead of Aura when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assassinate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your sneak attacks deal additional damage. You can spend a Prep Point to enter stealth, even from combat or while in plain sight, and can do so outside your turn in combat. Sneak attacks that incapacitate an enemy do not break stealth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convincing Fake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration, Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose a Skill you have no points in, and raise it to half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate. You can use “Assume a Disguise” without spending Prep Points.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infiltration Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. You can use a Prep Point to prevent you or your allies from being revealed when they otherwise would be. “Assume a Disguise” also produces disguises for your allies. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iocane Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Stealth, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your sneak attacks can put targets to sleep and wipe away their short-term memory when they would otherwise incapacitate. Successfully taking out a target in this way recovers a Prep Point. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shadowdancing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can move your shadow independently of your body. Your shadow can interact with physical objects, including moving objects and attacking enemies, but takes your action to do so. It can move roughly as far as you can see, but cannot enter brightly lit areas. You can spend a Prep Point to switch places with your shadow. You see perfectly in the dark.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spycraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“Assume a Disguise” is nearly instantaneous, and allows you to adopt an alias with a legally documented background and history. “What You Needed” can produce forgeries of documents, symbols of authority, and similar items. “I Know a Guy” can be used to produce blackmail on targets. You can open any non-magical lock.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swashbuckler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Eres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can counterattack or move after successfully defending against an attack. You can spend a Prep Point to succeed at defending against an attack regardless of your roll. You can move before and after taking an action in combat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Forteiza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional Physical box. You can convert a Prep Point into Physical box or vice versa, and can do so once per action while in combat. You do not need to sleep, and cannot be rendered unconscious, though you may be incapacitated through other means.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Loquit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning as though it were Aura, Bravery, or Knowledge for social purposes. You can spend a Prep Point to reroll any social action you take, up to one additional time. You can use “I Know A Guy” without spending Prep Points.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Siva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning or Agility to provoke and intimidate in combat. When you succeed on provoking or intimidating an enemy in combat, you recover a Prep Point.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Tuco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can steal from, or disarm, a target on a successful attack or defense. You can spend a Prep Point to inflict a sneak attack regardless of stealth. Using an item as an action does not end your turn in combat, though subsequent uses will.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arta Valar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks can target Mental health instead of Physical. You can spend a Prep Point to take an action before someone else, including taking actions outside of your turn in combat. You can use this ability a maximum of one time between your normal turns in combat. Whenever there’s a question of who goes first, the answer is you.</t>
+    <t xml:space="preserve">Allows for control and limited manifestation of plant matter. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can speak with and understand beasts. You can use "I Know a Guy" to recruit a local beast to aid you. The beast can track, fight, and is capable of anything that a creature of its kind might otherwise do. The beast will follow your orders, but will prioritize its own survival. Only one beast can be recruited at a time.</t>
   </si>
   <si>
     <t xml:space="preserve">Soldier</t>
   </si>
   <si>
-    <t xml:space="preserve">Discipline</t>
+    <t xml:space="preserve">Fencer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Social, Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique inflicts a box of Mental damage on successful attacks, in addition to any Physical damage dealt. You have Advantage when using Bravery to provoke others, in or out of combat. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inner Flame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At any time when you would otherwise spend a Fortune Point, you can spend a Physical box instead. When you recover Physical or Mental boxes, you recover one more than you would otherwise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sharpshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique lowers the difficulty of making precise attacks, such as disarming a target by striking their hand. You have Advantage when making ranged attacks without any distractions. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spellbreak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique allows your attacks to destroy magic and spirits. You have Advantage when defending against magical attacks. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subvert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique delays the target’s turn on successful attacks, in addition to any Physical damage dealt. On a successful defense against a melee attack, you inflict a point of Physical damage on the attacker. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique extends the range of your attacks. Melee attacks create blades of wind, while ranged attacks are followed by gusts of wind. You have Advantage when defending against ranged attacks. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guardian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When an ally would otherwise take damage, you can spend a Fortune Point to negate it, so long as you are able to provide a narrative justification for how you do so. You can use Strength or Bravery to detect danger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospitaler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can spend a Fortune Point to revive an incapacitated ally, clearing one box of the appropriate damage track (but not their Injuries). This takes an action if done in combat. You can use Strength or Bravery to perform medical tasks. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you successfully intimidate a group of enemies, they take a box of Mental damage in addition to any other effects that intimidation may have. You have Advantage when using Bravery to intimidate in or out of combat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Will</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional Mental box. You can convert a Fortune Point into a Mental box or vice versa, and can do so as an action while in combat. You are immune to Mental damage from exhaustion, fear, or similar effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique provides Advantage to one nearby ally on their next roll in combat when you make a successful attack, in addition to dealing Physical damage to an enemy. You have Advantage when using Bravery to inspire or rally others outside of combat. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique allows your attacks to forcibly reposition targets, pushing them backwards or knocking in addition to any Physical damage dealt. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myrmidon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique allows your attacks to damage enemies or objects adjacent to your target, in addition to any Physical damage dealt to the original target. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gambler’s Fallacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treat a roll of 1 as a +0 instead of a -2. You recover a Fortune Point when you roll a 1.</t>
   </si>
   <si>
     <t xml:space="preserve">Iron Blood</t>
   </si>
   <si>
-    <t xml:space="preserve">Combat, Exploration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You are immune to most environmental hazards, including magical and alchemical hazards. You can spend a Fortune Point to weaponize an environmental hazard, such as sweeping a weapon through an open flame and sending fire at your enemies. Poisons, diseases, and similar afflictions have no effect on you. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Circle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take a free attack against enemies that attempt to enter or leave your melee range. You can spend a Fortune Point to prevent nearly anything from moving past you. You are immune to sneak attacks and similar effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Stance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can defend against Physical attacks and hazards using Bravery or Physique. You can spend a Fortune Point to negate an attack against a nearby ally. You cannot be moved, knocked down, or otherwise repositioned against your will.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Star</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks also count as a rally for one ally of your choice, requiring no additional rolls when the attack is successful. You can spend a Fortune Point to revive an incapacitated ally using a rally. When you recover Physical or Mental health, you recover one more box than you would otherwise.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Strength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks land with brutal force, dealing additional Physical damage when the attack is successful. You can spend a Fortune Point to perform a feat of incredible strength, such as bending metal bars or picking up a cart. You take Advantage on any roll that relies on brute strength.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Will</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional Mental box. You can convert a Fortune Point into a Mental box or vice versa, and can do so once per action while in combat. You are immune to Mental damage from exhaustion, fear, psychological attacks, or similar effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fortune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Those you provoke or intimidate are prone to bouts of misfortune. The next roll against them, from you or your allies, has Advantage. You can spend a Fortune Point to change this effect into a lasting weakness affiliated with a specific threat (fire, blades, heartbreak, poverty, etc.) Rolls related to this threat have Advantage against the target.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gambler’s Fallacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You recover a Fortune Point when you roll a 1. You can spend a Fortune Point to guarantee a 10 on your next action without rolling. You win all games of chance as though by divine intervention.</t>
+    <t xml:space="preserve">You are immune to most poisons and diseases. Take Advantage against environmental hazards, traps, and area of effect attacks.</t>
   </si>
   <si>
     <t xml:space="preserve">Lucky</t>
   </si>
   <si>
-    <t xml:space="preserve">Gain an additional two Fortune Point boxes. When you use a Fortune Point to reroll, add a +1 to the reroll result. When a roll for luck is called, the result is always favorable for you.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near Miss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you roll a 1 you take a +0 instead of a -2 to the result. You can spend a Fortune Point to avoid taking damage from an attack or hazard. When you would otherwise be taken out, you can roll. On a 9 or higher, you miraculously avoid being incapacitated.</t>
+    <t xml:space="preserve">Gain an additional two Fortune Points. When a roll for luck is called for, it always goes in your favor.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Chance</t>
   </si>
   <si>
-    <t xml:space="preserve">Bend probability in your favor or against others. You can spend a Fortune Point to use Physique or Bravery instead of Aura when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Winning Charm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You make a good first impression, acquiring the respect or affection of people you meet. You can spend a Fortune Point to establish a reputation of your choice among those you meet for the first time, regardless of whether or not it’s deserved. You have Advantage when using Bravery or Physique to impress others.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hordebreaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks affect anyone or anything near your target, becoming area-of-effect. You can spend a Fortune Point to make an attack against every enemy in combat, or to strike one target twice in a single action. Take Advantage when attacking a group of similar enemies (i.e. a pack of wolves).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skybreaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks, both melee and ranged, have a much longer range than normal. You can spend a Fortune Point to make a difficult shot with pinpoint accuracy. When you tie attacking an enemy, you succeed instead of the defender.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spellbreaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks can damage spells and spirits. You can spend a Fortune Point to deflect a spell back at its caster or clear away magical effects in the area. Take Advantage when attacking mages or spirits.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stancebreaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks force enemies to reposition and volley objects into the air. You can spend a Fortune Point to manipulate a target’s placement; knocking it down, pinning it in place, launching it into the air, or throwing it a great distance. Enemies that you hit have reduced movement throughout combat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swordbreaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks can strike through stone and metal, damaging equipment and piercing cover as well as causing harm. You can spend a Fortune Point to outright destroy an object or obstacle. Take Advantage when attacking armored or very large enemies.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Willbreaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks also count as a provocation or intimidation for one enemy, requiring no additional rolls to produce either effect when successful and dealing additional Mental damage. You can spend a Fortune Point to provoke or intimidate all enemies in combat. Recover a Fortune Point when you incapacitate an enemy that you’ve previously provoked or intimidated.</t>
+    <t xml:space="preserve">Manipulate probability and tweak the odds. Used to alter the likelihood of events. You can spend a Fortune Point to use Physique or Bravery instead of Aura when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using this technique allows your attacks to deal an additional box of Physical damage, on top of any Physical damage that would otherwise be dealt. You can expend a Fortune Point on a successful attack to make it especially destructive, breaking through metal, armor, and similarly durable materials. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
   </si>
 </sst>
 </file>
@@ -932,8 +935,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FF272727"/>
+          <fgColor rgb="FFDEDEDE"/>
+          <bgColor rgb="FF18191D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1012,16 +1015,16 @@
   </sheetPr>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E66" activeCellId="0" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.64"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="37.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="155.45"/>
   </cols>
   <sheetData>
@@ -1070,10 +1073,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1084,13 +1087,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1101,10 +1104,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>17</v>
@@ -1121,10 +1124,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1135,13 +1138,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1149,16 +1152,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1166,16 +1169,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1183,16 +1186,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1200,16 +1203,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1217,16 +1220,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1234,16 +1237,16 @@
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1251,16 +1254,16 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1268,16 +1271,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1285,16 +1288,16 @@
         <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1302,16 +1305,16 @@
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1319,16 +1322,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1336,625 +1339,625 @@
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="E20" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="C21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="C22" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="E22" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="C23" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="C24" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="E24" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="C25" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>89</v>
-      </c>
       <c r="D33" s="9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="14" t="s">
         <v>100</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B39" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="13" t="s">
-        <v>105</v>
-      </c>
       <c r="D39" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>119</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>133</v>
+        <v>57</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B51" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>141</v>
-      </c>
       <c r="D51" s="13" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C53" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C54" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E54" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C55" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="13" t="s">
         <v>149</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="E55" s="14" t="s">
         <v>150</v>
@@ -1988,10 +1991,10 @@
         <v>156</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2002,13 +2005,13 @@
         <v>152</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2019,13 +2022,13 @@
         <v>152</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2036,13 +2039,13 @@
         <v>152</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2053,13 +2056,13 @@
         <v>152</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2067,13 +2070,13 @@
         <v>151</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>170</v>
@@ -2084,16 +2087,16 @@
         <v>151</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>171</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2101,16 +2104,16 @@
         <v>151</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2118,16 +2121,16 @@
         <v>151</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2135,16 +2138,16 @@
         <v>151</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2152,13 +2155,13 @@
         <v>151</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="E67" s="18" t="s">
         <v>182</v>
@@ -2175,7 +2178,7 @@
         <v>184</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>185</v>
@@ -2192,10 +2195,10 @@
         <v>186</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2206,13 +2209,13 @@
         <v>183</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2223,13 +2226,13 @@
         <v>183</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2240,13 +2243,13 @@
         <v>183</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2257,13 +2260,13 @@
         <v>183</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to kits
</commit_message>
<xml_diff>
--- a/miracuse_kits.xlsx
+++ b/miracuse_kits.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="198">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Exploration, Alchemy, Potion, Substance</t>
   </si>
   <si>
-    <t xml:space="preserve">Adopt an animal-like adaption for a short period of time by drinking a potion. Example of effects could include a cat’s night vision, a bat’s sense of hearing, or a gecko’s skin. Can be used as a substance to attract monsters.</t>
+    <t xml:space="preserve">Adopt an animal-like adaption for a short period of time by drinking a potion. Example of effects could include a cat’s night vision, a bat’s sense of hearing, or a gecko’s skin. Can be used as a substance to attract animals and monsters.</t>
   </si>
   <si>
     <t xml:space="preserve">Elixir</t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Recovery, Alchemy, Potion</t>
   </si>
   <si>
-    <t xml:space="preserve">Recover from harm and illness by drinking a potion. This can include recovering Physical damage, recovering Mental damage, treating an Injury, or curing various natural afflictions. </t>
+    <t xml:space="preserve">Recover from harm and illness by drinking a potion. This can include recovering Physical damage, recovering Mental damage, treating an Injury, or curing various natural afflictions. Can be used to revitilize most living creatures.</t>
   </si>
   <si>
     <t xml:space="preserve">Faerie Fire</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Combat, Exploration, Alchemy, Substance, Grenade</t>
   </si>
   <si>
-    <t xml:space="preserve">Create dazzling fireworks displays with a highly volatile powder. Capable of producing blinding lights, making smoke screens, emitting deafening noises, and causing wracking coughs when breathed. Can be used as a grenade to produce any two of the effects listed or inflict Physical damage.</t>
+    <t xml:space="preserve">Create dazzling fireworks displays with a highly volatile powder. Capable of producing blinding lights, making smoke screens, emitting deafening noises, and causing painful coughing when breathed. Can be used as a grenade to produce any two of the effects listed or inflict Physical damage.</t>
   </si>
   <si>
     <t xml:space="preserve">Golden Silk</t>
@@ -106,22 +106,22 @@
     <t xml:space="preserve">Exploration, Alchemy, Tool</t>
   </si>
   <si>
-    <t xml:space="preserve">A sigil that allows the user to see and hear around the object it’s applied to for two days. Can be used to create a shikigami, a paper oragami servant capable of flight and relaying messages. The shikigami falls apart after twenty-four hours, or when this Kit is removed. </t>
+    <t xml:space="preserve">A sigil that allows the user to see and hear around the object it’s applied to for two hours. Can be used to create a shikigami, a paper origami servant capable of flight and relaying messages. The shikigami falls apart after twenty-four hours, or when this Kit is removed. </t>
   </si>
   <si>
     <t xml:space="preserve">Rune of Featherweight</t>
   </si>
   <si>
-    <t xml:space="preserve">A sigil that halves the weight of objects for two hours when applied. Can be used to create a bag that’s bigger on the inside than the outside, capable of holding three times its volume without growing heavier. The bag falls apart after twenty-four hours, or when this Kit is removed.</t>
+    <t xml:space="preserve">A sigil that makes objects lighter and more brittle for two hours when applied. Can be used to create a backpack that’s bigger on the inside than the outside, capable of holding three times its volume without growing heavier. The bag falls apart after twenty-four hours, or when this Kit is removed.</t>
   </si>
   <si>
     <t xml:space="preserve">Rune of Quickening</t>
   </si>
   <si>
-    <t xml:space="preserve">A sigil that makes solid objects malleable for a short period of time when applied. Can be used to create a quicksilver familiar, a sentient metal ooze that can reshape itself into tools and weapons on command. The familiar hardens into whatever shape it was holding after two hours.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rune of Strength</t>
+    <t xml:space="preserve">A sigil that makes solid objects malleable and liquid for a short period of time when applied. Can be used to create a quicksilver familiar, a sentient metal ooze that can reshape itself into tools and weapons on command. The familiar hardens into whatever shape it was holding after two hours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rune of Stoneweight</t>
   </si>
   <si>
     <t xml:space="preserve">Combat, Exploration, Alchemy, Tool</t>
@@ -133,16 +133,16 @@
     <t xml:space="preserve">Spirit of Animation</t>
   </si>
   <si>
-    <t xml:space="preserve">Magic, Alchemy, Tool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Awaken and imbue with purpose. Used to compel objects to move with a life of their own. You can spend this Kit’s uses to use Knowledge or Perception when using this spirit.</t>
+    <t xml:space="preserve">Spirit, Alchemy, Tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awaken inanimate objects, compel them to move and act on your orders. You can spend this Kit’s Charges to use Knowledge or Perception when using this spirit.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Transmutation</t>
   </si>
   <si>
-    <t xml:space="preserve">Transform and alter. Used to change the properties of a substance, such as shape and weight. The greater the difference from the original, the more difficult the change. You can spend this Kit’s uses to use Knowledge or Perception when using this spirit.</t>
+    <t xml:space="preserve">Change the properties of a substance, such as shape and weight. The greater the difference from the original, the more difficult the change. You can spend this Kit’s Charges to use Knowledge or Perception when using this spirit.</t>
   </si>
   <si>
     <t xml:space="preserve">Sapper</t>
@@ -152,447 +152,6 @@
   </si>
   <si>
     <t xml:space="preserve">Combat, Alchemy, Grenade, Bullet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that is especially destructive, dealing two boxes of Physical damage and damaging the surrounding area. When used as a bullet, deals two boxes of Physical damage and pierces through obstacles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electromagnetic Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with crackling electricity, or magnetizes an area, forcing metal objects in the vicinity to adhere to one another. When used as a bullet, deals two boxes of Physical damage and one of the grenade effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friction Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with a grease slick, or a quick-drying adhesive. When used as a bullet, deals two boxes of Physical damage and one of the grenade effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermic Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with roaring flames, or a layer of ice. When used as a bullet, deals two boxes of Physical damage and one of the grenade effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trenchsteel Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with metal ball bearings, or a sprawl of barbed wire. When used as a bullet, ricochets in closed spaces, deals two boxes of Physical damage, and can change course mid-flight by detonating a second time .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vapor Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area in tear gas, or a billowing cloud of fog. When used as a bullet, can instantly rust through most metals.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Abjuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seal and purify. Used to create barriers and dispel magic.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Divination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seek and learn. Used to scry for hidden things and reveal new information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speak and understand. Used to commune with all creatures and compel others to your will.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Necromancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corrupt and wrong. Used to raise the dead and curse the living.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Restoration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recovery, Magic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restore and repair. Used to heal wounds and mend broken objects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Summoning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petition and conjure. Used to pull otherworldly influences into the mortal realm.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Aether</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of electricity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of air.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Earth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of earth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Flame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of flame.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Metal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of metal and magnetism.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of water.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wizard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Binding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adhere and restrain. Used to lash things together with gravitational force.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Entropy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diminish and dissolve. Used to unravel targets into their base elements.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Force</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel raw magical energy. Used to lob bolts of force at enemies, or otherwise manipulate energy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Locomotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accelerate and slow. Used to manipulate kinetic energy, adding or taking away speed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Reinforcement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fortify and empower. Used to improve existing qualities, such as making someone stronger or faster.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Thermos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heat and cool. Used to manipulate thermal energy, adding or taking away temperature.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoundrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assassin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assassinate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your sneak attacks deal an additional box of Physical damage. You can use "Assume a Disguise" to disappear from sight, taking an action to do so if done in combat. You can tell if a target will be incapacitated by your sneak attack before you make it.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convincing Fake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration, Social, Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choose a Skill and raise it to half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate. You can use “Assume a Disguise” without spending Prep Points.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infiltration Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. When you use "Assume a Disguise", you can provide disguises to your allies as well. When you or an ally would otherwise be revealed, you can spend a Prep Point to prevent it, so long as you can narratively describe how you do so.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iocane Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Social, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your sneak attacks can put targets to sleep and cause short-term memory loss. You can use "What You Needed" to produce a vial of liquid that makes those who drink it highly suggestible. Those under the effects of the liquid will speak truthfully, but are visibly drugged, and slow to react.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pin Down</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Technique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks reduce an enemy’s movement, cutting off their ability to escape or pursue. Using this technique greatly reduces a target’s mobility, in addition to any Physical damage dealt.  You can expend a Prep Point to amplify this technique or combine this with another.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Shadow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magic, Stealth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Obscure and muffle. Used to manipulate darkness and quiet footsteps. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charm Arcana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning as though it were Presence, Bravery, or Knowledge for social purposes. You can spend a Prep Point to reroll a social action and take the new result, a maximum of one time per social action. You can use "I Know a Guy" without spending Prep Points.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lore Arcana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Cunning or Agility to detect and identify magic. You can use "What You Needed" to produce an item that briefly channels or negates magic you've identified. You can use Cunning or Agility when recalling information about history, religion, magic, or politics.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resilience Arcana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health, Exploration, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional Physical box. You can exchange Mental boxes for Prep Points and vice versa, and can do so as an action while in combat. You do not need to sleep, and cannot be rendered unconscious against your will, but can be incapacitated in other ways.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brighten and bend light. Used to create and manipulate illusory images, as well as to see afar. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Sound</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amplify and distort. Used to create and manipulate sound, as well as to listen in from a distance. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">War Arcana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your fighting style resembles dancing, making you particularly mobile. Using this technique allows you to move before and after making an attack. You can spend a Prep Point to take an additional action on your turn, besides another attack. You can expend a Prep Point to combine this technique with another.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ranger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herbalism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use “What You Needed” to produce teas and poultices, capable of recovering Physical or Mental boxes outside of combat. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prepared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration, Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional two Prep Points. When you use a Prep Point to change Kits, you can change two Kits instead of one.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quickdraw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks are swift and silent, preventing targets from crying out when struck or otherwise making noise. Using this technique ensures that an enemy won’t cause a commotion for a brief period of time, in addition to any Physical damage dealt. You always go first when turn order is described. You can expend a Prep Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allows for control and limited manifestation of plants. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tamer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration, Social</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can speak with and understand beasts. You can use "I Know a Guy" to recruit a local beast to aid you. The beast can track, fight, and is capable of anything that a creature of its kind might otherwise do. The beast will follow your orders, but will prioritize its own survival. Only one beast can be recruited at a time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twin Strike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks hit two targets instead of one. Using this technique gives your attack an additional target, with both hits landing within moments of one another. You can expend a Prep Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soldier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fencer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Called Shot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration, Technique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks are exceptionally precise. Using this technique lowers the difficulty of making targeted attacks, such as disarming an enemy by striking their hand or blinding an enemy by striking their eyes. You have Advantage when making ranged attacks without any distractions. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Social, Technique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks taunt and frustrate targets in addition to dealing damage. Using this technique inflicts a box of Mental damage on successful attacks, in addition to any Physical damage dealt. You have Advantage when using Bravery to provoke others. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inner Flame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At any time when you would otherwise spend a Fortune Point, you can spend a Physical box instead. When you recover Physical or Mental boxes, you recover one more than you would otherwise.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riposte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On a successful defense against a melee attack, you inflict a box of Physical damage to the attacker. You recover a Fortune Point when an enemy is incapacitated using this Kit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spellbreak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks interfere with magic. Using this technique allows your attacks to destroy spells and spirits. You have Advantage when defending against magical attacks. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind Strike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your melee attacks create blades of cutting wind, while your ranged attacks are propelled by gusts. Using this technique greatly extends the range of your attacks. You have Advantage when defending against ranged attacks. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When an ally would otherwise take damage, you can spend a Fortune Point to negate it, so long as you are able to provide a narrative justification for how you do so. You can use Strength or Bravery to detect danger.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hospitaler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can spend a Fortune Point to revive an incapacitated ally, restoring one box of either of their damage tracks and taking your action to do so if done in combat. You can use Strength or Bravery to perform medical tasks outside of combat, giving you the ability to heal others and treat injuries. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks demand the attention of targets and cloud their perception. Using this technique compels an enemy to focus on you on successful attacks, in addition to any Physical damage dealt. You have Advantage when using Bravery to intimidate others. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Will</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gain an additional Mental box. You can convert a Fortune Point into a Mental box or vice versa, and can do so as an action while in combat. You are immune to Mental damage from exhaustion, fear, or similar effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks encourage and inspire allies on the battlefield. Using this technique can provide Advantage to one nearby ally on their next roll in combat when you make a successful attack, in addition to dealing Physical damage to an enemy. You have Advantage when using Bravery to inspire or rally others outside of combat. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks strike with enough force to knock targets back or topple them over. Using this technique allows your attacks to forcibly reposition enemies, in addition to any Physical damage dealt. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myrmidon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cleave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks are especially destructive, hitting enemies and objects adjacent to your target. Using this technique allows your attacks to inflict Physical damage in an area of effect. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gambler’s Fallacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treat a roll of 1 as a -1 instead of a -2. You recover a Fortune Point when you roll a 1 in combat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Strike</t>
   </si>
   <si>
     <r>
@@ -603,7 +162,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Your attacks cause harm even on glancing blows. Using this techique allows your attacks to inflict damage even when your roll would normally have tied with the defender. You can expend a Fortune Point to guarantee a hit, so long as hitting the target is within the realm of possibility. </t>
+      <t xml:space="preserve">Grenade that is especially destructive, dealing two boxes of Physical damage and damaging the surrounding area. When used as a bullet, </t>
     </r>
     <r>
       <rPr>
@@ -612,8 +171,574 @@
         <rFont val="Fira Sans"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+      <t xml:space="preserve">deals an additional box of Physical damage</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and pierces through obstacles.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Electromagnetic Charges</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Grenade that covers an area with crackling electricity, or magnetizes an area, forcing metal objects in the vicinity to adhere to one another. When used as a bullet, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deals an additional box of Physical damage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and one of the grenade effects.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Friction Charges</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Grenade that covers an area with a grease slick, or a quick-drying adhesive. When used as a bullet, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deals an additional box of Physical damage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and one of the grenade effects.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermic Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenade that covers an area with roaring flames, or a layer of ice. When used as a bullet, deals an additional box of Physical damage and one of the grenade effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trenchsteel Charges</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Grenade that covers an area with metal ball bearings, or a sprawl of barbed wire. When used as a bullet, ricochets in closed spaces, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deals an additional box of Physical damage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and can change course mid-flight by detonating a second time .</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Vapor Charges</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Grenade that covers an area in tear gas, or a billowing cloud of fog. When used as a bullet, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deals an additional box of Physical damage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and can instantly rust through most metals.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Abjuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create barriers, dispel magic, and repel otherworldly influences.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Divination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration, Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find people, places, things, and hidden knowledge through divination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social, Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speak all languages, use charm magic, and compel others to your will.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Necromancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raise the dead, curse the living, and meddle with the boundary between life and death.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Restoration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recovery, Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heal Physical wounds, restore broken objects, and treat natural afflictions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Summoning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration, Social, Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call imps, pixies, and other minor magical creatures to serve you. Pull otherworldly influences into the world. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Aether</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate electricity, shoot lightning, and stun enemies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate air, create gusts of wind, and fall gently.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate earth, reshape terrain, and mold stone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Flame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate fire, throw flames, and ignite objects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate metal, create magnetic fields, and sharpen blades.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate water, freeze liquids, and conjure fog.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wizard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Binding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate bonds, adhering things together or loosening them from one another.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Entropy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate decay, accelerating or slowing processes like rotting and rusting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate magic energy, lob bolts of raw power at enemies, and tinker with magical forces present in the world.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Locomotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate kinetic energy, add or reduce speed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Gravity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate gravity, add or reduce weight.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Thermos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate thermal energy, add or reduce heat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scoundrel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assassin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assassinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your sneak attacks deal an additional box of Physical damage. You can use "Assume a Disguise" to disappear from sight, taking an action to do so if done in combat. You can tell if a target will be incapacitated by your sneak attack before you make it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convincing Fake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration, Social, Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose a Skill and raise it to half the level of your highest Skill (rounded down). You can spend a Prep Point to change the chosen Skill, provided you have a few minutes to concentrate. You can use “Assume a Disguise” without spending Prep Points.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infiltration Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. When you use "Assume a Disguise", you can provide disguises to your allies as well. When you or an ally would otherwise be revealed, you can spend a Prep Point to prevent it, so long as you can narratively describe how you do so.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks reduce an enemy’s movement, cutting off their ability to escape or pursue. Using this technique greatly reduces a target’s mobility, in addition to any Physical damage dealt. You have Advantage when using Agility to sprint, as might be the case when chasing after someone or retreating from danger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Technique, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks strike at an enemy’s nerves. Using this technique can incapacitate targets without lasting harm or visible injury, in addition to any Physical damage dealt. You have Advantage when sensing the motivations of others, such as detecting lies, by picking up on nervous ticks or other tells.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Shadow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit, Stealth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate shadows, obscure appearances, and blind enemies. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charm Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning as though it were Presence, Bravery, or Knowledge for social purposes. You can spend a Prep Point to reroll a social action and take the new result, a maximum of one time per social action. You can use "I Know a Guy" without spending Prep Points.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use Cunning or Agility to detect and identify magic. You can use "What You Needed" to produce an item that briefly channels or negates magic you've identified. You can use Cunning or Agility when recalling information about history, religion, magic, or politics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resilience Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health, Exploration, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional Physical box. You can exchange Mental boxes for Prep Points and vice versa, and can do so as an action while in combat. You do not need to sleep, and cannot be rendered unconscious against your will, but can be incapacitated in other ways.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate light, create ghostly illusions, and see afar. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate sound, shatter eardrums, and eavesdrop from afar. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">War Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your fighting style resembles dancing, making you particularly mobile. Using this technique allows you to move before and after making an attack, escaping from melee range or otherwise covering ground. You have Advantage reacting to traps or similar surprise attacks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbalism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can use “What You Needed” to heal Physical and Mental damage outside of combat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration, Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Prep Points. When you use a Prep Point to change Kits, you can change two Kits instead of one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quickdraw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are swift and silent, preventing targets from crying out when struck or otherwise making noise. Using this technique ensures that an enemy won’t cause a commotion for a brief period of time, in addition to any Physical damage dealt. You have Advantage when determining who acts first, including combat turn order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate plants, encourage growth, and influence the environment. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Social</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can speak with and understand beasts. You can use "I Know a Guy" to recruit a local beast to aid you. The beast can track, fight, and is capable of anything that a creature of its kind might otherwise do. The beast will follow your orders, but will prioritize its own survival. Only one beast can be recruited at a time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twin Strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks hit two targets instead of one. Using this technique gives your attack an additional target, with both hits landing within moments of one another. The additional target cannot be the same as the original target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fencer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Called Shot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are exceptionally precise. Using this technique allows you to harm specific targets (like eyes or hands), in addition to any Physical damage dealt. You have Advantage when making ranged attacks without any distractions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Social, Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks taunt and frustrate targets in addition to dealing damage. Using this technique inflicts a box of Mental damage on successful attacks, in addition to any Physical damage dealt. You have Advantage when using Bravery to provoke others. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inner Flame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At any time when you would otherwise spend a Fortune Point, you can spend a Physical box instead. When you recover Physical or Mental boxes, you recover one more than you would otherwise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riposte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On a successful defense against a melee attack, you inflict a box of Physical damage to the attacker. You recover a Fortune Point when an enemy is incapacitated using this Kit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spellbreak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks interfere with magic. Using this technique allows your attacks to destroy spells and spirits, in addition to any Physical damage dealt. You have Advantage when defending against magical attacks. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind Strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your melee attacks create blades of cutting wind, while your ranged attacks are propelled by gusts. Using this technique greatly extends the range of your attacks. You have Advantage when defending against projectile attacks like arrows and bullets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guardian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When an ally would otherwise take damage, you can spend a Fortune Point to negate it, so long as you are able to provide a narrative justification for how you do so. You can use Strength or Bravery to detect danger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospitaler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can spend a Fortune Point to revive an incapacitated ally, restoring one box of either of their damage tracks and taking your action to do so if done in combat. You can use Strength or Bravery to perform medical tasks outside of combat, giving you the ability to heal Physical damage and treat Physical injuries. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks demand the attention of targets and cloud their perception. Using this technique compels an enemy to focus on you on successful attacks, in addition to any Physical damage dealt. You have Advantage when using Bravery to intimidate others.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Will</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional Mental box. You can convert a Fortune Point into a Mental box or vice versa, and can do so as an action while in combat. You are immune to Mental damage from exhaustion, fear, or similar effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks encourage and inspire allies on the battlefield. Using this technique can provide Advantage to one nearby ally on their next roll in combat when you make a successful attack, in addition to dealing Physical damage to an enemy. You have Advantage when using Bravery to inspire or rally others outside of combat. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks strike with enough force to knock targets back or topple them over. Using this technique allows your attacks to forcibly reposition enemies, in addition to any Physical damage dealt. You have Advantage against any attempt to forcibly move you and against any effect that impedes your movement, including terrain hazards like ice or mud.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myrmidon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are especially destructive, hitting enemies and objects adjacent to your target. Using this technique allows your attacks to inflict damage in a small area of effect. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gambler’s Fallacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treat any roll of 1 as a -1 instead of a -2. You recover a Fortune Point when you roll a 1 in combat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Blow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks cause harm even on glancing blows. Using this techique allows your attacks to inflict damage when your roll would normally have tied with the defender, increasing the odds of a successful attack. You have Advantage when performing feats that rely solely on raw muscle, such as lifting heavy objects or bending metal bars.</t>
   </si>
   <si>
     <t xml:space="preserve">Lucky</t>
@@ -625,13 +750,13 @@
     <t xml:space="preserve">Spirit of Chance</t>
   </si>
   <si>
-    <t xml:space="preserve">Manipulate probability and tweak the odds. Used to alter the likelihood of events. You can spend a Fortune Point to use Physique or Bravery instead of Aura when using this spirit.</t>
+    <t xml:space="preserve">Manipulate probability, tweak the odds in your favor, and jinx enemies. You can spend a Fortune Point to use Physique or Bravery instead of Aura when using this spirit.</t>
   </si>
   <si>
     <t xml:space="preserve">Sunder</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks are brutally effective, causing great harm and striking through armor. Using this technique allows your attacks to deal an additional box of Physical damage when successful. You have Advantage when using Strength to destroy obstacles. You can expend a Fortune Point to combine this technique with another, or amplify its effects.</t>
+    <t xml:space="preserve">Your attacks are brutally effective, causing great harm and striking through armor. Using this technique allows your attacks to deal an additional box of Physical damage when successful. You have Advantage when using this technique to destroy objects and obstacles. </t>
   </si>
 </sst>
 </file>
@@ -834,7 +959,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -880,6 +1005,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1043,8 +1172,8 @@
   </sheetPr>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E70" activeCellId="0" sqref="E70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1475,10 +1604,10 @@
         <v>71</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1486,16 +1615,16 @@
         <v>54</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1503,16 +1632,16 @@
         <v>54</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1520,16 +1649,16 @@
         <v>54</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1537,16 +1666,16 @@
         <v>54</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1554,16 +1683,16 @@
         <v>54</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1571,16 +1700,16 @@
         <v>54</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1588,16 +1717,16 @@
         <v>54</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>88</v>
+        <v>66</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1605,16 +1734,16 @@
         <v>54</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1622,16 +1751,16 @@
         <v>54</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1639,16 +1768,16 @@
         <v>54</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1656,16 +1785,16 @@
         <v>54</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1673,628 +1802,628 @@
         <v>54</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>66</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" s="13" t="s">
+      <c r="A38" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="B38" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="C38" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="D38" s="15" t="s">
         <v>103</v>
       </c>
+      <c r="E38" s="16" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="13" t="s">
+      <c r="A39" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" s="14" t="s">
+      <c r="B39" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="D39" s="15" t="s">
         <v>106</v>
       </c>
+      <c r="E39" s="16" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="13" t="s">
+      <c r="A40" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" s="14" t="s">
+      <c r="B40" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="D40" s="15" t="s">
         <v>109</v>
       </c>
+      <c r="E40" s="16" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" s="13" t="s">
+      <c r="A41" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" s="14" t="s">
+      <c r="B41" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="D41" s="15" t="s">
         <v>112</v>
       </c>
+      <c r="E41" s="16" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="13" t="s">
+      <c r="A42" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="14" t="s">
+      <c r="B42" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="D42" s="15" t="s">
         <v>115</v>
       </c>
+      <c r="E42" s="16" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" s="13" t="s">
+      <c r="A43" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" s="14" t="s">
+      <c r="B43" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="D43" s="15" t="s">
         <v>118</v>
       </c>
+      <c r="E43" s="16" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="14" t="s">
+      <c r="A44" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="C44" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="D44" s="15" t="s">
         <v>122</v>
       </c>
+      <c r="E44" s="16" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="14" t="s">
+      <c r="A45" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="D45" s="15" t="s">
         <v>125</v>
       </c>
+      <c r="E45" s="16" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="D46" s="14" t="s">
+      <c r="A46" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="D46" s="15" t="s">
         <v>128</v>
       </c>
+      <c r="E46" s="16" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D47" s="14" t="s">
+      <c r="A47" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E47" s="15" t="s">
-        <v>130</v>
+      <c r="E47" s="16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D48" s="14" t="s">
+      <c r="A48" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>132</v>
+      <c r="E48" s="16" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E49" s="15" t="s">
+      <c r="A49" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>134</v>
       </c>
+      <c r="D49" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C50" s="14" t="s">
+      <c r="A50" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="C50" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="D50" s="15" t="s">
         <v>138</v>
       </c>
+      <c r="E50" s="16" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D51" s="14" t="s">
+      <c r="A51" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="D51" s="15" t="s">
         <v>141</v>
       </c>
+      <c r="E51" s="16" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E52" s="15" t="s">
+      <c r="A52" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="15" t="s">
         <v>143</v>
       </c>
+      <c r="D52" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D53" s="14" t="s">
+      <c r="A53" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E53" s="15" t="s">
-        <v>145</v>
+      <c r="E53" s="16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D54" s="14" t="s">
+      <c r="A54" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="D54" s="15" t="s">
         <v>148</v>
       </c>
+      <c r="E54" s="16" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E55" s="15" t="s">
+      <c r="A55" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="15" t="s">
         <v>150</v>
       </c>
+      <c r="D55" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B56" s="17" t="s">
+      <c r="A56" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="B56" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="C56" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="D56" s="19" t="s">
         <v>155</v>
       </c>
+      <c r="E56" s="20" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B57" s="17" t="s">
+      <c r="A57" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C57" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D57" s="18" t="s">
+      <c r="B57" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C57" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="D57" s="19" t="s">
         <v>158</v>
       </c>
+      <c r="E57" s="20" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B58" s="17" t="s">
+      <c r="A58" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C58" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D58" s="18" t="s">
+      <c r="B58" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="D58" s="19" t="s">
         <v>161</v>
       </c>
+      <c r="E58" s="20" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B59" s="17" t="s">
+      <c r="A59" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C59" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D59" s="18" t="s">
+      <c r="B59" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="D59" s="19" t="s">
         <v>164</v>
       </c>
+      <c r="E59" s="20" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B60" s="17" t="s">
+      <c r="A60" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C60" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E60" s="19" t="s">
+      <c r="B60" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="19" t="s">
         <v>166</v>
       </c>
+      <c r="D60" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B61" s="17" t="s">
+      <c r="A61" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C61" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E61" s="19" t="s">
+      <c r="B61" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="19" t="s">
         <v>168</v>
       </c>
+      <c r="D61" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C62" s="18" t="s">
+      <c r="A62" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B62" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="D62" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="E62" s="19" t="s">
+      <c r="C62" s="19" t="s">
         <v>171</v>
       </c>
+      <c r="D62" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="D63" s="18" t="s">
+      <c r="A63" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="D63" s="19" t="s">
         <v>174</v>
       </c>
+      <c r="E63" s="20" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="E64" s="19" t="s">
+      <c r="A64" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C64" s="19" t="s">
         <v>176</v>
       </c>
+      <c r="D64" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="E65" s="19" t="s">
+      <c r="A65" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" s="19" t="s">
         <v>178</v>
       </c>
+      <c r="D65" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="E66" s="19" t="s">
+      <c r="A66" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>180</v>
       </c>
+      <c r="D66" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E67" s="19" t="s">
+      <c r="A67" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C67" s="19" t="s">
         <v>182</v>
       </c>
+      <c r="D67" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C68" s="18" t="s">
+      <c r="A68" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="D68" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E68" s="19" t="s">
+      <c r="C68" s="19" t="s">
         <v>185</v>
       </c>
+      <c r="D68" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="D69" s="18" t="s">
+      <c r="A69" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C69" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="D69" s="19" t="s">
         <v>188</v>
       </c>
+      <c r="E69" s="20" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="E70" s="19" t="s">
+      <c r="A70" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C70" s="19" t="s">
         <v>190</v>
       </c>
+      <c r="D70" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C71" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="E71" s="19" t="s">
+      <c r="A71" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C71" s="19" t="s">
         <v>192</v>
       </c>
+      <c r="D71" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="D72" s="18" t="s">
+      <c r="A72" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="D72" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E72" s="19" t="s">
-        <v>194</v>
+      <c r="E72" s="20" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="34.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E73" s="19" t="s">
+      <c r="A73" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C73" s="19" t="s">
         <v>196</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E73" s="20" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redid character sheet in React
</commit_message>
<xml_diff>
--- a/miracuse_kits.xlsx
+++ b/miracuse_kits.xlsx
@@ -8,10 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1_2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$E$73</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$E$73</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1_2!$A$1:$E$73</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="273">
   <si>
     <t xml:space="preserve">Class</t>
   </si>
@@ -43,157 +45,622 @@
     <t xml:space="preserve">Alchemist</t>
   </si>
   <si>
+    <t xml:space="preserve">Enchanter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bag of Holding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have a bag that’s bigger on the inside than the outside, capable of reducing the weight of objects placed within. You can expend a Charge Point to place a particularly large or heavy object within. The object should generally be less than 300 lbs. and less than five times the bag’s size.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have a golem made from clay, capable of fighting and lifting heavy objects. The golem has a Strength equal to half your Knowledge rounded down. You can expend a Charge Point to create an additional golem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Charge Points. When you Produce a Potion, the potion restores an additional box of Physical damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quicksilver Familiar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alchemy, Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have a familiar made from liquid metal, capable of shaping itself into weapons, tools, and objects. You can expend a Charge Point to deflect an attack by having the familiar change into a shield or similar object.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shikigami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have a servant made from enchanted paper, capable of flying, spying, and carrying messages. The shikigami has a Cunning equal to half your Knowledge rounded down. You can expend a Charge Point to create an additional servant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awaken inanimate objects, compel them to move and act on your orders. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Called Shot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are exceptionally precise. Using this technique allows you to harm specific targets (like eyes or hands), in addition to any Physical damage dealt. You have Advantage when making ranged attacks without any distractions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electromagnetic Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition are electrically charged, shocking or magnetizing targets in addition to any Physical damage dealt. When used with Produce a Grenade inflicts Physical damage and one other effect in a wide area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friction Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition involve capsules of liquid, producing quick-drying adhesive or slippery grease in addition to any Physical damage dealt. When used with Produce a Grenade this kit inflicts Physical damage and one other effect in a wide area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermic Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition have thermal properties, producing flames or frost on targets in addition to any Physical damage dealt. When used with Produce a Grenade this kit inflicts Physical damage and one other effect in a wide area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trenchsteel Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition are physically loaded, exploding into a mass of ball bearings or barbed wire in addition to any Physical damage dealt. When used with Produce a Grenade this kit inflicts Physical damage and one other effect in a wide area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vapor Charges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition are chemically loaded, instantly rusting through metal or producing small clouds of tear gas in addition to any Physical damage dealt. When used with Produce a Grenade this kit inflicts Physical damage and one other effect in a wide area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmuter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmute Division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Separate objects. Can be used to physically sever two objects from one another, or to distill an object into its base elements. The more complex the intended result is, the more difficult the change. Requires physical contact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmute Self</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alchemy, Resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expend a Mental box to recover a Physical box or vice versa. Can only be applied to yourself. When done in combat, requires an action.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmute Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reshape an object, altering its form by expanding or contracting its mass. Requires physical contact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmute Strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strengthen an object, making it harder and more durable. Or weaken an object, making it flimsy and more brittle. Requires physical contact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmute Substance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convert one material into another. The greater the difference from the original, the more difficult the change. Requires physical contact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmute Synthesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combine objects. Can be used to physically weld two objects to one another, or to mix them into one another as a means of creating a new object. The more complex the intended result is, the more difficult the change. Requires physical contact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Abjuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit, Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create barriers, dispel magic, and repel otherworldly influences. You can expend a Mana Point to deflect an attack aimed at you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Divination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find people, places, things, and hidden knowledge through divination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicate with all creatures, use charm magic, and compel others to your will.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Necromancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raise the dead, curse the living, and meddle with the boundary between life and death.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Restoration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heal Physical wounds, restore broken objects, and treat natural afflictions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Summoning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pull otherworldly influences into the world. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shaman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Aether</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate electricity, create lightning, and stun enemies. Represents emptiness and void.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate air, create gusts of wind, and fall gently. Represents movement and freedom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate earth, reshape terrain, and mold stone. Represents solidity and strength.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Flame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate fire, conjure flames, and blast enemies. Represents cleansing and destruction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate metal, magnetize metallic objects, and sharpen or dull blades. Represents clarity and reason.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate water, conjure fog, and freeze liquids. Represents tranquility and adaptability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wizard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manafont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Mana Points. When you Sacrifice a Mental health box, you gain two Mana Points instead of one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Entropy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate decay, accelerating or decelerating processes like rotting and rusting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Force</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Perform limited telekinesis, levitating objects and lobbing them through the air. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">You can expend a Mana Point to deflect an attack aimed at you.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Gravity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate gravity, add or reduce weight.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Locomotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate kinetic energy, add or reduce speed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Thermos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate thermal energy, add or reduce heat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scoundrel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assassin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golden Silk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A potent hallucinogenic. Can be used to induce confusion, to put a target into a stupor, to render someone highly suggestable, or to inflict Mental damage. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manifold Venom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A collection of dangerous poisons. Can be applied to the user’s weapons to induce paralysis, sap strength, create nausea, cause blindness, or inflict additional Physical damage. Requires an action if applied in combat, unless the Kit is amplified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks reduce an enemy’s movement, cutting off their ability to escape or pursue. Using this technique greatly reduces a target’s mobility, in addition to any Physical damage dealt. You have Advantage when using Agility to sprint, as might be the case when chasing after someone or retreating from danger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks strike at an enemy’s nerves. Using this technique can incapacitate targets without lasting harm or visible injury, in addition to any Physical damage dealt. You have Advantage when sensing the motivations of others, such as detecting lies, by picking up on nervous ticks or other tells.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Shadow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate shadows, obscure appearances, and blind enemies. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncanny Dodge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can expend a Prep Point to avoid harm from an attack or hazard. You have Advantage against traps and area of effect attacks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faerie Fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A volatile powder used in fireworks. Can create plumes of smoke, bright lights, flames, loud noises, or induce violent coughing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A specially treated water that negates magic. Can be used to counter spells, disperse spirits, damage magical objects, or repel monsters. You can expend a Prep Point to negate hostile magic as a reaction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resilience Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional Physical box. You do not need to sleep, and cannot be rendered unconscious against your will, but can be incapacitated in other ways.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate light, create ghostly illusions, and see afar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate sound, shatter eardrums, and eavesdrop from afar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">War Arcana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your fighting style resembles dancing, making you particularly mobile. Using this technique allows you to take a second action after making an attack, so long as the second action is not an attack. Examples might include moving out of range, using an item, or using magic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beast Balm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A mixture that bewitches animals. You can communicate with and befriend beasts. You can use I Know a Guy to recruit a local beast to aid you. The beast can track, fight, and is capable of anything that a creature of its kind might otherwise do. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beast’s Blood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A mixture that heightens senses. Can provide a bat’s sense of hearing, a hound’s sense of smell, or similar effects. When amplified, can provide more drastic animal adaptations, like fireproof scales or a fish’s gills. Can also be used to attract beasts and monsters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Prep Points.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quickdraw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are swift and silent, preventing targets from crying out when struck. Using this technique ensures that an enemy won’t cause a commotion for a brief period of time, in addition to any Physical damage dealt. You have Advantage when determining who acts first, including combat turn order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate plants, encourage growth, and influence the environment. Represents growth and vitality. Can be used to accelerate the process of natural healing outside of combat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twin Strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks hit two targets instead of one. Using this technique gives your attack an additional target, with both hits landing within moments of one another. The additional target cannot be the same as the original target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fencer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aura Strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your melee attacks create blades of cutting wind, while your ranged attacks are propelled by gusts. Using this technique greatly extends the range of your attacks. You have Advantage when defending against projectile attacks like arrows and bullets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your melee attacks bend the shape of your weapon in unpredictable ways, while your ranged attacks can change trajectory in mid-flight. Using this technique allows your attacks to circumvent cover and obstacles. When you tie with a defender while attacking, you deal damage regardless.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flourish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are complex, dazzling, and distracting to enemies. Using this technique can either give Disadvantage to the target’s next action, or give Advantage to the next attack made on the target. You have Advantage when using Bravery to inspire or rally others.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks unnerve and frustrate targets in addition to dealing damage. Using this technique inflicts a box of Mental damage on successful attacks, in addition to any Physical damage dealt. You have Advantage when using Bravery to provoke others. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inner Flame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At any time when you would otherwise spend a Fortune Point, you can spend a Physical box instead. When you recover Physical or Mental boxes, you recover one more than you would otherwise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riposte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On a successful defense against a melee attack, you inflict a box of Physical damage to the attacker. You recover a Fortune Point when an enemy is incapacitated in this fashion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guardian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a nearby ally would otherwise take damage, you can take damage in their place, so long as you are able to provide a narrative justification for how you do so. You recover a Fortune Point when using this Kit. You cannot attempt to block, dodge, or otherwise reduce damage taken using this Kit. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospitaler Salts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alchemy, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revive an incapacitated ally and allow them to briefly ignore the effects of their injuries. Revived allies clear one box of damage, Physical or Mental, depending on which is necessary. Requires physical contact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks demand the attention of targets and cloud their perception. Using this technique compels an enemy to focus on you after a successful attack, in addition to any Physical damage dealt. You have Advantage when using Bravery to intimidate others.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron Will</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional Mental box. You are immune to Mental damage from exhaustion, fear, or similar psychological effects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks strike with enough force to knock targets around or launch them into the air. Using this technique allows your attacks to forcibly reposition enemies, in addition to any Physical damage dealt. You have Advantage against any attempt to forcibly move you, and against any effect that impedes your movement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spellbreak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks interfere with magic. Using this technique allows your attacks to destroy spells and spirits, in addition to any Physical damage dealt. You have Advantage when defending against magical attacks. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myrmidon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blitz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are more likely to cause harm. Using this technique adds +1 to the roll result of your attacks, significantly improving the chance that they’ll inflict damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are especially destructive, hitting enemies and objects adjacent to your target. Using this technique allows your attacks to inflict damage in a small area of effect. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danger Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enemies that attempt to leave your melee range take one box of Physical damage. You recover a Fortune Point when an enemy is incapacitated in this fashion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lucky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Fortune Points. When you use a Fortune Point to reroll, take the better result of the two rolls.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit of Chance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipulate probability, tweak the odds in your favor, and jinx enemies. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your attacks are brutally effective, causing great harm and breaking through defences. Using this technique allows your attacks to cut or pierce durable materials like stone and metal. Successful attacks also deal an additional box of Physical damage. You have Advantage when using this technique to destroy objects and obstacles. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Chemist</t>
   </si>
   <si>
-    <t xml:space="preserve">Beast’s Blood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration, Alchemy, Potion, Substance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adopt an animal-like adaption for a short period of time by drinking a potion. Examples of effects could include a cat’s night vision, a bat’s sense of hearing, or a gecko’s skin. Can be used as a substance to attract animals and monsters.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elixir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recovery, Alchemy, Potion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recover from harm and illness by drinking a potion. Can be used to recover Physical damage, recover Mental damage, treat an injury, or cure various natural afflictions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Faerie Fire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration, Alchemy, Substance, Grenade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create dazzling fireworks displays with a highly volatile powder. Capable of producing blinding lights, making smoke screens, emitting deafening noises, or causing painful coughing when breathed. Can be used as a grenade to produce one of the effects listed and inflict Physical damage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Golden Silk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration, Social, Alchemy, Substance, Grenade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distort perceptions with a potent hallucionegic. Can be used to induce confusion, to put others into a stupor, to provide Advantage against Mental attacks, or to make targets highly suggestible. Can be used as a grenade to produce one of the effects listed or inflict Mental damage. Can be used as an offering to powerful spirits and supernatural creatures.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holy Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration, Alchemy, Substance, Grenade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neutralize magical energy with treated water. Can be used to counter spells, disperse spirits, damage magical objects, nullify magical effects, or repel monsters. Can be used as a grenade to produce all of the listed effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manifold Venom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inflict debilitating effects with a collection of dangerous poisons. Can be used to induce paralysis, sap strength, create nausea, or cause blindness. Can be used as a grenade to produce one of the effects listed or inflict Physical damage. Can be applied to weapons to provide one of the effects listed on the next successful attack, in addition to any damage dealt by the attack.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enchanter</t>
+    <t xml:space="preserve">Exploration, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A mixture that heightens senses. Can provide a bat’s sense of hearing, a hound’s sense of smell, or similar effects. When amplified, can provide more drastic animal adaptations, like fireproof scales or a fish’s gills. Can also be used to attract animals and monsters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A volatile powder used in fireworks. Can create plumes of smoke, bright lights, flames, loud noises, or induce violent coughing. When used with Produce a Grenade inflicts Physical damage and one other effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Social, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A potent hallucinogenic. Can be used to induce confusion, to put a target into a stupor, to render someone highly suggestable, or to inflict Mental damage. When used with Produce a Grenade inflicts Mental damage and one other effect. Can also be used as an offering to powerful spirits and supernatural creatures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A specially treated water that negates magic. Can be used to counter spells, disperse spirits, damage magical objects, or repel monsters. When used with Produce a Grenade produces all such effects at once. Can also be used to destroy the undead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A collection of dangerous poisons. Can be applied to the user’s weapons to induce paralysis, sap strength, create nausea, cause blindness, or inflict additional Physical damage. When used with Produce a Grenade inflicts Physical damage and one other effect. Can also be used to carefully burn through durable materials as a potent acid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gain an additional two Charge Points. When you use a Charge Point to Produce a Potion, you produce two instead of one.</t>
   </si>
   <si>
     <t xml:space="preserve">Rune of Awareness</t>
   </si>
   <si>
-    <t xml:space="preserve">Exploration, Alchemy, Tool</t>
-  </si>
-  <si>
     <t xml:space="preserve">A sigil that allows the user to see and hear around the object it’s applied to for two hours. Can be used to create a shikigami, a paper origami servant capable of flight and relaying messages. The shikigami falls apart after twenty-four hours, or when this Kit is removed. </t>
   </si>
   <si>
     <t xml:space="preserve">Rune of Featherweight</t>
   </si>
   <si>
-    <t xml:space="preserve">A sigil that makes objects lighter and more brittle for two hours when applied. Can be used to create a backpack that’s bigger on the inside than the outside, capable of holding three times its volume without growing heavier. The bag falls apart after twenty-four hours, or when this Kit is removed.</t>
+    <t xml:space="preserve">A sigil that makes objects lighter and more brittle for a short time. When amplified, can be used to create a backpack that’s bigger on the inside than the outside, capable of holding three times its volume without growing heavier. The bag falls apart after twenty-four hours, or when this Kit is removed.</t>
   </si>
   <si>
     <t xml:space="preserve">Rune of Quickening</t>
   </si>
   <si>
-    <t xml:space="preserve">A sigil that makes solid objects malleable and liquid for two minutes when applied. Can be used to create a quicksilver familiar, a sentient metal ooze that can reshape itself into tools and weapons on command. The familiar hardens into whatever shape it was holding after two hours.</t>
+    <t xml:space="preserve">A sigil that makes solid objects malleable and liquid for a short time. When amplified, can be used to create a quicksilver familiar, a sentient metal ooze that can reshape itself into tools and weapons on command. The familiar hardens into whatever shape it was holding after twenty-four hours, when this Kit is removed, or at the user’s discretion.</t>
   </si>
   <si>
     <t xml:space="preserve">Rune of Stoneweight</t>
   </si>
   <si>
-    <t xml:space="preserve">Combat, Exploration, Alchemy, Tool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A sigil that makes objects stronger and heavier for two hours when applied. Can be used to create a golem from stone or dirt, which will follow your orders and fight on your behalf for two hours.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Animation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit, Alchemy, Tool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Awaken inanimate objects, compel them to move and act on your orders. You can spend this Kit’s Charges to use Knowledge or Perception when using this spirit.</t>
+    <t xml:space="preserve">A sigil that makes objects stronger and heavier for a short time. When amplified, can be used to create a golem from stone or dirt, which will follow your orders and fight on your behalf for twenty-four hours, or when this Kit is removed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awaken inanimate objects, compel them to move and act on your orders. You can spend a Charge Point to use Knowledge or Perception when using this spirit.</t>
   </si>
   <si>
     <t xml:space="preserve">Spirit of Transmutation</t>
   </si>
   <si>
-    <t xml:space="preserve">Change the properties of a substance, such as shape and weight. The greater the difference from the original, the more difficult the change. You can spend this Kit’s Charges to use Knowledge or Perception when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sapper</t>
+    <t xml:space="preserve">Change the properties of a substance, such as shape and weight. The greater the difference from the original, the more difficult the change. You can spend a Charge Point to use Knowledge or Perception when using this spirit.</t>
   </si>
   <si>
     <t xml:space="preserve">Concussive Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Combat, Alchemy, Grenade, Bullet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that is especially destructive, dealing two boxes of Physical damage and damaging the surrounding area. When used as a bullet, deals an additional box of Physical damage and pierces through obstacles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electromagnetic Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with crackling electricity, or magnetizes an area, forcing metal objects in the vicinity to adhere to one another. When used as a bullet, deals an additional box of Physical damage and one of the grenade effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friction Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with a grease slick, or a quick-drying adhesive. When used as a bullet, deals an additional box of Physical damage and one of the grenade effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thermic Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with roaring flames, or a sheet of frost. When used as a bullet, deals an additional box of Physical damage and one of the grenade effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trenchsteel Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area with metal ball bearings, or a sprawl of barbed wire. When used as a bullet, ricochets in closed spaces, deals an additional box of Physical damage, and can change course mid-flight by detonating a second time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vapor Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grenade that covers an area in tear gas, or a billowing cloud of fog. When used as a bullet, deals an additional box of Physical damage and can instantly rust through most metals.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Abjuration</t>
+    <t xml:space="preserve">Combat, Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition have unusual materials, ricocheting in closed spaces or detonating while in the air to change trajectory. Deals two points of Physical damage to everything in range when used with Produce a Grenade.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition are electrically charged, shocking or magnetizing targets in addition to any Physical damage dealt. When used with Produce a Grenade inflicts Physical damage and one other effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition have capsules of liquid, producing quick-drying adhesive or slippery grease in addition to any Physical damage dealt. When used with Produce a Grenade inflicts Physical damage and one other effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition have thermal properties, producing flames or ice on targets in addition to any Physical damage dealt. When used with Produce a Grenade inflicts Physical damage and one other effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition are physically loaded, exploding into a mass of ball bearings or barbed wire in addition to any Physical damage dealt. When used with Produce a Grenade inflicts Physical damage and one other effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attacks that use this ammunition are chemically loaded, instantly rusting through metal or producing small clouds of tear gas in addition to any Physical damage dealt. When used with Produce a Grenade inflicts Physical damage and one other effect.</t>
   </si>
   <si>
     <t xml:space="preserve">Combat, Exploration, Spirit</t>
@@ -202,132 +669,39 @@
     <t xml:space="preserve">Create barriers, dispel magic, and repel otherworldly influences.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Divination</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exploration, Spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">Find people, places, things, and hidden knowledge through divination.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Language</t>
-  </si>
-  <si>
     <t xml:space="preserve">Social, Spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">Communicate with all creatures, use charm magic, and compel others to your will.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Necromancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raise the dead, curse the living, and meddle with the boundary between life and death.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Restoration</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recovery, Spirit</t>
   </si>
   <si>
-    <t xml:space="preserve">Heal Physical wounds, restore broken objects, and treat natural afflictions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Summoning</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exploration, Social, Spirit</t>
   </si>
   <si>
     <t xml:space="preserve">Call imps, pixies, and other minor magical creatures to serve you. Pull otherworldly influences into the world. </t>
   </si>
   <si>
-    <t xml:space="preserve">Shaman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Aether</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manipulate electricity, create lightning, and stun enemies. Represents emptiness and divinity.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manipulate air, create gusts of wind, and fall gently. Represents movement and freedom.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Earth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manipulate earth, reshape terrain, and mold stone. Represents solidity and strength.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Flame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manipulate fire, conjure flames, and blast enemies. Represents cleansing and destruction.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Metal</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manipulate metal, magnetize metallic objects, and sharpen metal. Represents clarity and reason.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manipulate water, conjure fog, and freeze liquids. Represents tranquility and adaptability.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wizard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Entropy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manipulate decay, accelerating processes like rotting and rusting.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Force</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manipulate magical energy, lob bolts of force at enemies, and create forcefields.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Gravity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manipulate gravity, add or reduce weight.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Locomotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manipulate kinetic energy, add or reduce speed.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spirit of Siphoning</t>
   </si>
   <si>
     <t xml:space="preserve">Manipulate lifeforce, steal Physical health from others, or bequeath your own.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Thermos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manipulate thermal energy, add or reduce heat.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoundrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assassin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Assassinate</t>
   </si>
   <si>
@@ -355,36 +729,18 @@
     <t xml:space="preserve">Nearby allies can use your Cunning when moving in stealth. When you use Assume a Disguise, you can provide disguises to your allies as well. When you or an ally would otherwise be revealed, you can spend a Prep Point to prevent it, so long as you can narratively describe how you do so.</t>
   </si>
   <si>
-    <t xml:space="preserve">Pin Down</t>
-  </si>
-  <si>
     <t xml:space="preserve">Combat, Technique</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks reduce an enemy’s movement, cutting off their ability to escape or pursue. Using this technique greatly reduces a target’s mobility, in addition to any Physical damage dealt. You have Advantage when using Agility to sprint, as might be the case when chasing after someone or retreating from danger.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressure Points</t>
-  </si>
-  <si>
     <t xml:space="preserve">Combat, Technique, Stealth</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks strike at an enemy’s nerves. Using this technique can incapacitate targets without lasting harm or visible injury, in addition to any Physical damage dealt. You have Advantage when sensing the motivations of others, such as detecting lies, by picking up on nervous ticks or other tells.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Shadow</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spirit, Stealth</t>
   </si>
   <si>
     <t xml:space="preserve">Manipulate shadows, obscure appearances, and blind enemies. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
   </si>
   <si>
-    <t xml:space="preserve">Bard</t>
-  </si>
-  <si>
     <t xml:space="preserve">Charm Arcana</t>
   </si>
   <si>
@@ -403,60 +759,33 @@
     <t xml:space="preserve">You have a perfect memory while this Kit is equipped, capable of recalling minute details or committing a book to memory in minutes. You can use What You Needed to recall information in place of a Knowledge roll. </t>
   </si>
   <si>
-    <t xml:space="preserve">Resilience Arcana</t>
-  </si>
-  <si>
     <t xml:space="preserve">Health, Recovery</t>
   </si>
   <si>
     <t xml:space="preserve">Gain an additional Physical box. You can exchange Mental boxes for Prep Points and vice versa, and can do so as an action while in combat. You do not need to sleep, and cannot be rendered unconscious against your will, but can be incapacitated in other ways.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Light</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manipulate light, create ghostly illusions, and see afar. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Sound</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manipulate sound, shatter eardrums, and eavesdrop from afar. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
   </si>
   <si>
-    <t xml:space="preserve">War Arcana</t>
-  </si>
-  <si>
     <t xml:space="preserve">Your fighting style resembles dancing, making you particularly mobile. Using this technique allows you to move before and after making an attack, escaping from melee range or otherwise covering ground. You have Advantage when reacting to traps or similar surprise attacks.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ranger</t>
-  </si>
-  <si>
     <t xml:space="preserve">Herbalism</t>
   </si>
   <si>
     <t xml:space="preserve">Recovery</t>
   </si>
   <si>
-    <t xml:space="preserve">You can use What You Needed to heal Physical and Mental damage outside of combat. You are immune to all poisons, diseases, and similar effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prepared</t>
+    <t xml:space="preserve">You can use What You Needed to heal Physical damage outside of combat. You are immune to all poisons, diseases, and similar effects.</t>
   </si>
   <si>
     <t xml:space="preserve">Gain an additional two Prep Points. When you use a Prep Point to change Kits, you can change two Kits instead of one.</t>
   </si>
   <si>
-    <t xml:space="preserve">Quickdraw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks are swift and silent, preventing targets from crying out when struck. Using this technique ensures that an enemy won’t cause a commotion for a brief period of time, in addition to any Physical damage dealt. You have Advantage when determining who acts first, including combat turn order.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spirit of Wood</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manipulate plants, encourage growth, and influence the environment. Represents growth and vitality. You can spend a Prep Point to use Cunning or Agility when using this spirit.</t>
   </si>
   <si>
@@ -469,67 +798,28 @@
     <t xml:space="preserve">You can speak with and understand beasts. You can use I Know a Guy to recruit a local beast to aid you. The beast can track, fight, and is capable of anything that a creature of its kind might otherwise do. The beast will follow your orders, but will prioritize its own survival. Only one beast can be recruited at a time.</t>
   </si>
   <si>
-    <t xml:space="preserve">Twin Strike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks hit two targets instead of one. Using this technique gives your attack an additional target, with both hits landing within moments of one another. The additional target cannot be the same as the original target.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soldier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fencer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Called Shot</t>
-  </si>
-  <si>
     <t xml:space="preserve">Combat, Exploration, Technique</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks are exceptionally precise. Using this technique allows you to harm specific targets (like eyes or hands), in addition to any Physical damage dealt. You have Advantage when making ranged attacks without any distractions. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harass</t>
-  </si>
-  <si>
     <t xml:space="preserve">Combat, Social, Technique</t>
   </si>
   <si>
-    <t xml:space="preserve">Your attacks unnerve and frustrate targets in addition to dealing damage. Using this technique inflicts a box of Mental damage on successful attacks, in addition to any Physical damage dealt. You have Advantage when using Bravery to provoke others. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inner Flame</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At any time when you would otherwise spend a Fortune Point, you can spend a Physical box instead. When you recover Physical or Mental boxes, you recover one more than you would otherwise.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riposte</t>
-  </si>
-  <si>
     <t xml:space="preserve">Combat</t>
   </si>
   <si>
-    <t xml:space="preserve">On a successful defense against a melee attack, you inflict a box of Physical damage to the attacker. You recover a Fortune Point when an enemy is incapacitated in this fashion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spellbreak</t>
-  </si>
-  <si>
     <t xml:space="preserve">Your attacks interfere with magic. Using this technique allows your attacks to harm spells and spirits, in addition to any Physical damage dealt. You have Advantage when defending against magical attacks. </t>
   </si>
   <si>
     <t xml:space="preserve">Wind Strike</t>
   </si>
   <si>
-    <t xml:space="preserve">Your melee attacks create blades of cutting wind, while your ranged attacks are propelled by gusts. Using this technique greatly extends the range of your attacks. You have Advantage when defending against projectile attacks like arrows and bullets.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardian</t>
+    <t xml:space="preserve">Field Medic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combat, Exploration, Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can spend a Fortune Point to revive an incapacitated ally, restoring one box of either of their damage tracks and taking your action to do so if done in combat. </t>
   </si>
   <si>
     <t xml:space="preserve">Combat, Exploration</t>
@@ -538,24 +828,6 @@
     <t xml:space="preserve">When an ally would otherwise take damage, you can spend a Fortune Point to negate it, so long as you are able to provide a narrative justification for how you do so. You can use Strength or Bravery to detect danger.</t>
   </si>
   <si>
-    <t xml:space="preserve">Hospitaler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combat, Exploration, Recovery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You can use Strength or Bravery to perform medical tasks outside of combat, giving you the ability to heal Physical damage and treat Physical injuries. You can spend a Fortune Point to revive an incapacitated ally, restoring one box of either of their damage tracks and taking your action to do so if done in combat. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks demand the attention of targets and cloud their perception. Using this technique compels an enemy to focus on you after a successful attack, in addition to any Physical damage dealt. You have Advantage when using Bravery to intimidate others.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron Will</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gain an additional Mental box. You can convert a Fortune Point into a Mental box or vice versa, and can do so as an action while in combat. You are immune to Mental damage from exhaustion, fear, or similar effects.</t>
   </si>
   <si>
@@ -565,21 +837,9 @@
     <t xml:space="preserve">Your attacks encourage and inspire allies on the battlefield. Using this technique can provide Advantage to one nearby ally on their next roll in combat when you make a successful attack, in addition to dealing Physical damage to an enemy. You have Advantage when using Bravery to inspire or rally others outside of combat. </t>
   </si>
   <si>
-    <t xml:space="preserve">Smite</t>
-  </si>
-  <si>
     <t xml:space="preserve">Your attacks strike with enough force to knock targets around or topple them over. Using this technique allows your attacks to forcibly reposition enemies, in addition to any Physical damage dealt. You have Advantage against any attempt to forcibly move you, and against any effect that impedes your movement, including terrain hazards like ice or mud.</t>
   </si>
   <si>
-    <t xml:space="preserve">Myrmidon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cleave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your attacks are especially destructive, hitting enemies and objects adjacent to your target. Using this technique allows your attacks to inflict damage in a small area of effect. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Gambler’s Fallacy</t>
   </si>
   <si>
@@ -595,19 +855,10 @@
     <t xml:space="preserve">Your attacks cause harm even on glancing blows. Using this techique allows your attacks to succeed when your roll would normally have tied with the defender. You have Advantage when performing feats that rely solely on raw muscle, such as lifting heavy objects or bending metal bars.</t>
   </si>
   <si>
-    <t xml:space="preserve">Lucky</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gain an additional two Fortune Points. When a roll for luck is called for, it always goes in your favor.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spirit of Chance</t>
-  </si>
-  <si>
     <t xml:space="preserve">Manipulate probability, tweak the odds in your favor, and jinx enemies. You can spend a Fortune Point to use Physique or Bravery instead of Aura when using this spirit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunder</t>
   </si>
   <si>
     <t xml:space="preserve">Your attacks are brutally effective, causing great harm and striking through armor. Using this technique allows your attacks to deal an additional box of Physical damage when successful. You have Advantage when using this technique to destroy objects and obstacles. </t>
@@ -621,7 +872,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -681,6 +932,12 @@
       <name val="Fira Sans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Fira Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1009,6 +1266,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1016,8 +1277,8 @@
   </sheetPr>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1074,10 +1335,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1088,13 +1349,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1105,13 +1366,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1122,13 +1383,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1139,13 +1400,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1153,16 +1414,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1170,16 +1431,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1187,16 +1448,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1204,16 +1465,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1221,16 +1482,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1238,16 +1499,16 @@
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1255,16 +1516,16 @@
         <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1272,16 +1533,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="D15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1289,16 +1550,16 @@
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1306,16 +1567,16 @@
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1323,16 +1584,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1340,934 +1601,2208 @@
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="E20" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>80</v>
-      </c>
       <c r="D29" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="E34" s="11" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>93</v>
-      </c>
       <c r="D35" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="15" t="s">
         <v>99</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B41" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>110</v>
-      </c>
       <c r="D41" s="14" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>124</v>
+        <v>16</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>127</v>
+        <v>13</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B49" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>137</v>
+        <v>8</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>146</v>
+        <v>21</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>127</v>
+        <v>25</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>161</v>
+        <v>25</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="B63" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>171</v>
-      </c>
       <c r="D63" s="18" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>127</v>
+        <v>13</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="E67" s="19" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="E68" s="19" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>186</v>
+        <v>25</v>
       </c>
       <c r="E69" s="19" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>127</v>
+        <v>13</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B73" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E73"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E73"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="109.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>182</v>
       </c>
+    </row>
+    <row r="7" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>161</v>
+      </c>
       <c r="C73" s="18" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>153</v>
+        <v>251</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>195</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added info button styling, modified default kit options
</commit_message>
<xml_diff>
--- a/miracuse_kits.xlsx
+++ b/miracuse_kits.xlsx
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Trenchsteel Charges</t>
   </si>
   <si>
-    <t xml:space="preserve">Attacks that use this ammunition are physically loaded, exploding into a mass of ball bearings or barbed wire in addition to any Physical damage dealt. When used with Produce a Grenade this kit inflicts Physical damage and one other effect in a wide area.</t>
+    <t xml:space="preserve">Attacks that use this ammunition are physically loaded, exploding into a mass of ball bearings or coils of barbed wire in addition to any Physical damage dealt. When used with Produce a Grenade this kit inflicts Physical damage and one other effect in a wide area.</t>
   </si>
   <si>
     <t xml:space="preserve">Vapor Charges</t>
@@ -1833,8 +1833,8 @@
   </sheetPr>
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Added more documentation pages
</commit_message>
<xml_diff>
--- a/miracuse_kits.xlsx
+++ b/miracuse_kits.xlsx
@@ -54,10 +54,46 @@
     <t xml:space="preserve">Conjurer</t>
   </si>
   <si>
-    <t xml:space="preserve">Athame</t>
+    <t xml:space="preserve">Brimstone Powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alchemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An otherworldly dust that conducts and magnifies magical energy. When added to fire it becomes hellfire, burning hotter and creating a noxious stench. When you use Produce a Grenade, the resulting explosion deals an additional point of damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fey Venom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A chemical that can stem the flow of blood or increase the rate of blood loss depending on how the substance is prepared. When you Produce a Potion, it heals an additional Physical box.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solomon Rod</t>
   </si>
   <si>
     <t xml:space="preserve">Weapon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An metal rod that holds sway over otherworldly creatures. Wielding this weapon compels nearby magical creatures into obedience, providing Advantage on all rolls to influence them. Successful attacks against magical creatures deal one additional box of Mental damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talisman of Demons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talisman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A wand or other object that can be used to bring forth demonic influence. Can be used to summon imps, consult devils for knowledge, or fling hellfire. You have Advantage when using Knowledge to recall forbidden information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talisman of Fey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A wand or other object that can be used to bring forth faerie influence. Can be used to summon pixies, bewitch the senses, and change your appearence. You have Advantage when using Presence to confuse and bewilder others.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Talisman of Jinn</t>
   </si>
   <si>
     <r>
@@ -68,7 +104,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">A ritual dagger that conducts magical energy. Using this weapon restores a Mana Point whenever it’s used to incapacitate an enemy. </t>
+      <t xml:space="preserve">A wand or other object that can be used to bring forth jinn influence. Can be used to summon snakes, call forth hot desert wind, and see into the past of an object. </t>
     </r>
     <r>
       <rPr>
@@ -77,82 +113,10 @@
         <rFont val="Fira Sans"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">At any time when you would otherwise spend a Mana Point, you can spend a Physical box instead. </t>
+      <t xml:space="preserve">You have Advantage when using Knowledge to recall history.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Brimstone Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alchemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An otherworldly dust that conducts and magnifies magical energy. When added to fire it becomes hellfire, burning hotter and creating a noxious stench. When you use Produce a Grenade, the resulting explosion deals an additional point of damage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ironbrew</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A chemical that stem the flow of blood or increase the rate of blood loss depending on how the substance is prepared. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">When you Produce a Potion, it heals an additional Physical box.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Solomon Rod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An inscribed metal rod that holds sway over otherworldly creatures. Using this weapon compels magical creatures into obedience when touched, providing Advantage on all rolls afterwards to socially influence them. Successful attacks against magical creatures deal one additional box of Mental damage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Talisman of Demons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Talisman</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A wand or other object that can be used to bring forth demonic influence. Can be used to summon imps, consult devils for knowledge, or fling hellfire. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Fira Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">You have Advantage when using Knowledge to recall forbidden information.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Talisman of Fey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A wand or other object that can be used to bring forth faerie influence. Can be used to summon pixies, bewitch the senses, and change your appearence. You have Advantage when using Presence to confuse and bewilder others.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gunslinger</t>
   </si>
   <si>
@@ -207,10 +171,16 @@
     <t xml:space="preserve">A set of flexible gloves that have somehow been crafted out of finely worked adamantium. They protect the wearer’s hands from conditions as extreme as molten lava or caustic acid. You have Advantage when blocking attacks with the gloves.</t>
   </si>
   <si>
-    <t xml:space="preserve">Reshape Metal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reshape metal, altering its form by expanding or reducing its mass. The more drastic the change, the more difficult and time consuming it is. Requires physical contact. Can be completed instantaneously by expending a Charge Point.</t>
+    <t xml:space="preserve">Ring of Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A red ring with the power to convert metals into other metals. The greater the difference from the original, the more difficult the change. Requires physical contact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ring of Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A black ring with the power to reshape metal. The more drastic the change, the more difficult and time consuming it is. Requires physical contact. Can be completed instantaneously by expending a Charge Point.</t>
   </si>
   <si>
     <t xml:space="preserve">Runehammer</t>
@@ -225,12 +195,6 @@
     <t xml:space="preserve">A wand or other object that can be used to alter the properties of metals. Can be used to heat metals, purge them of impurities, and strengthen or weaken them.</t>
   </si>
   <si>
-    <t xml:space="preserve">Transmute Metal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convert one metal into another. The greater the difference from the original, the more difficult the change. Requires physical contact.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vitrolic Edge</t>
   </si>
   <si>
@@ -246,7 +210,7 @@
     <t xml:space="preserve">A metal chainlink whip engraved with warding runes. Using this weapon allows your attacks to interfere with magic, similar to a knight’s holy sword. The whip can be joined together to create a magic circle that repels magic from the outside and contains magic within.</t>
   </si>
   <si>
-    <t xml:space="preserve">Blinding Spear</t>
+    <t xml:space="preserve">Lantern Spear</t>
   </si>
   <si>
     <t xml:space="preserve">A shaft of steel tipped with enchanted silver that permanently glows with light. Using this weapon blinds creatures with strong night vision. Successful attacks against magical creatures deal an additional point of damage.</t>
@@ -2506,8 +2470,8 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2564,10 +2528,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2578,10 +2542,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>14</v>
@@ -2598,10 +2562,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2612,10 +2576,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>19</v>
@@ -2632,7 +2596,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>21</v>
@@ -2649,7 +2613,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>24</v>
@@ -2666,7 +2630,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>26</v>
@@ -2700,7 +2664,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>31</v>
@@ -2717,7 +2681,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>33</v>
@@ -2734,7 +2698,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>35</v>
@@ -2768,7 +2732,7 @@
         <v>40</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>41</v>
@@ -2802,7 +2766,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>45</v>
@@ -2819,7 +2783,7 @@
         <v>46</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>47</v>
@@ -2836,7 +2800,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>49</v>
@@ -2853,7 +2817,7 @@
         <v>51</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>52</v>
@@ -2870,7 +2834,7 @@
         <v>53</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>54</v>
@@ -2887,7 +2851,7 @@
         <v>55</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>56</v>
@@ -2904,7 +2868,7 @@
         <v>57</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>58</v>
@@ -2921,7 +2885,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>60</v>
@@ -2938,7 +2902,7 @@
         <v>61</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>62</v>
@@ -2955,7 +2919,7 @@
         <v>65</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>66</v>
@@ -2972,7 +2936,7 @@
         <v>67</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>68</v>
@@ -2989,7 +2953,7 @@
         <v>69</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>70</v>
@@ -3006,7 +2970,7 @@
         <v>71</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>72</v>
@@ -3023,7 +2987,7 @@
         <v>73</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>74</v>
@@ -3040,7 +3004,7 @@
         <v>75</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>76</v>
@@ -3057,7 +3021,7 @@
         <v>78</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>79</v>
@@ -3074,7 +3038,7 @@
         <v>80</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>81</v>
@@ -3108,7 +3072,7 @@
         <v>84</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>85</v>
@@ -3142,7 +3106,7 @@
         <v>89</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>90</v>
@@ -3159,7 +3123,7 @@
         <v>92</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>93</v>
@@ -3176,7 +3140,7 @@
         <v>94</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>95</v>
@@ -3193,7 +3157,7 @@
         <v>96</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E40" s="15" t="s">
         <v>97</v>
@@ -3210,7 +3174,7 @@
         <v>98</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E41" s="15" t="s">
         <v>99</v>
@@ -3227,7 +3191,7 @@
         <v>100</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>101</v>
@@ -3244,7 +3208,7 @@
         <v>102</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E43" s="15" t="s">
         <v>103</v>
@@ -3278,7 +3242,7 @@
         <v>109</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>110</v>
@@ -3295,7 +3259,7 @@
         <v>111</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>112</v>
@@ -3312,7 +3276,7 @@
         <v>113</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>114</v>
@@ -3329,7 +3293,7 @@
         <v>115</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>116</v>
@@ -3346,7 +3310,7 @@
         <v>117</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E49" s="19" t="s">
         <v>118</v>
@@ -3363,7 +3327,7 @@
         <v>120</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E50" s="19" t="s">
         <v>121</v>
@@ -3380,7 +3344,7 @@
         <v>122</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E51" s="19" t="s">
         <v>123</v>
@@ -3397,7 +3361,7 @@
         <v>124</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>125</v>
@@ -3414,7 +3378,7 @@
         <v>126</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E53" s="19" t="s">
         <v>127</v>
@@ -3431,7 +3395,7 @@
         <v>128</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>129</v>
@@ -3448,7 +3412,7 @@
         <v>130</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>131</v>
@@ -3465,7 +3429,7 @@
         <v>133</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E56" s="19" t="s">
         <v>134</v>
@@ -3499,7 +3463,7 @@
         <v>137</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>138</v>
@@ -3516,7 +3480,7 @@
         <v>139</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E59" s="19" t="s">
         <v>140</v>
@@ -3533,7 +3497,7 @@
         <v>141</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>142</v>
@@ -3550,7 +3514,7 @@
         <v>143</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>144</v>
@@ -3567,7 +3531,7 @@
         <v>147</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E62" s="23" t="s">
         <v>148</v>
@@ -3584,7 +3548,7 @@
         <v>149</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E63" s="23" t="s">
         <v>150</v>
@@ -3601,7 +3565,7 @@
         <v>151</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E64" s="23" t="s">
         <v>152</v>
@@ -3618,7 +3582,7 @@
         <v>153</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E65" s="23" t="s">
         <v>154</v>
@@ -3635,7 +3599,7 @@
         <v>155</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E66" s="23" t="s">
         <v>156</v>
@@ -3652,7 +3616,7 @@
         <v>157</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E67" s="23" t="s">
         <v>158</v>
@@ -3669,7 +3633,7 @@
         <v>160</v>
       </c>
       <c r="D68" s="22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E68" s="23" t="s">
         <v>161</v>
@@ -3686,7 +3650,7 @@
         <v>162</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E69" s="23" t="s">
         <v>163</v>
@@ -3703,7 +3667,7 @@
         <v>164</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E70" s="23" t="s">
         <v>165</v>
@@ -3737,7 +3701,7 @@
         <v>168</v>
       </c>
       <c r="D72" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E72" s="23" t="s">
         <v>169</v>
@@ -3754,7 +3718,7 @@
         <v>170</v>
       </c>
       <c r="D73" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E73" s="23" t="s">
         <v>171</v>
@@ -3771,7 +3735,7 @@
         <v>173</v>
       </c>
       <c r="D74" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E74" s="23" t="s">
         <v>174</v>
@@ -3788,7 +3752,7 @@
         <v>175</v>
       </c>
       <c r="D75" s="22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E75" s="23" t="s">
         <v>176</v>
@@ -3805,7 +3769,7 @@
         <v>177</v>
       </c>
       <c r="D76" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E76" s="23" t="s">
         <v>178</v>
@@ -3822,7 +3786,7 @@
         <v>179</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E77" s="23" t="s">
         <v>180</v>
@@ -3839,7 +3803,7 @@
         <v>181</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E78" s="23" t="s">
         <v>182</v>
@@ -3873,7 +3837,7 @@
         <v>187</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E80" s="27" t="s">
         <v>188</v>
@@ -3890,7 +3854,7 @@
         <v>189</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E81" s="27" t="s">
         <v>190</v>
@@ -3924,7 +3888,7 @@
         <v>194</v>
       </c>
       <c r="D83" s="26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E83" s="27" t="s">
         <v>195</v>
@@ -3941,7 +3905,7 @@
         <v>196</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E84" s="27" t="s">
         <v>197</v>
@@ -3975,7 +3939,7 @@
         <v>201</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E86" s="27" t="s">
         <v>202</v>
@@ -3992,7 +3956,7 @@
         <v>203</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E87" s="27" t="s">
         <v>204</v>
@@ -4009,7 +3973,7 @@
         <v>205</v>
       </c>
       <c r="D88" s="26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E88" s="27" t="s">
         <v>206</v>
@@ -4026,7 +3990,7 @@
         <v>207</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E89" s="27" t="s">
         <v>208</v>
@@ -4060,7 +4024,7 @@
         <v>211</v>
       </c>
       <c r="D91" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E91" s="27" t="s">
         <v>212</v>
@@ -4077,7 +4041,7 @@
         <v>214</v>
       </c>
       <c r="D92" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E92" s="27" t="s">
         <v>215</v>
@@ -4094,7 +4058,7 @@
         <v>216</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E93" s="27" t="s">
         <v>217</v>
@@ -4111,7 +4075,7 @@
         <v>218</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E94" s="27" t="s">
         <v>219</v>
@@ -4128,7 +4092,7 @@
         <v>220</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E95" s="27" t="s">
         <v>221</v>
@@ -4145,7 +4109,7 @@
         <v>222</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E96" s="27" t="s">
         <v>223</v>
@@ -4229,7 +4193,7 @@
         <v>227</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>228</v>
@@ -4263,7 +4227,7 @@
         <v>232</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="31" t="s">
         <v>233</v>
@@ -4297,7 +4261,7 @@
         <v>220</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>236</v>
@@ -4314,7 +4278,7 @@
         <v>237</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>238</v>
@@ -4450,7 +4414,7 @@
         <v>254</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>255</v>
@@ -4467,7 +4431,7 @@
         <v>256</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>257</v>
@@ -4518,7 +4482,7 @@
         <v>262</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E19" s="31" t="s">
         <v>263</v>
@@ -4654,7 +4618,7 @@
         <v>69</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E27" s="43" t="s">
         <v>280</v>
@@ -5195,7 +5159,7 @@
         <v>319</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>320</v>
@@ -5248,7 +5212,7 @@
         <v>324</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>325</v>
@@ -5282,7 +5246,7 @@
         <v>329</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>330</v>
@@ -5299,7 +5263,7 @@
         <v>331</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>332</v>
@@ -5316,7 +5280,7 @@
         <v>333</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>334</v>
@@ -5333,7 +5297,7 @@
         <v>335</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>336</v>
@@ -5346,7 +5310,7 @@
         <v>337</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>338</v>
@@ -5359,7 +5323,7 @@
         <v>339</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>340</v>
@@ -5372,7 +5336,7 @@
         <v>341</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>342</v>
@@ -5882,7 +5846,7 @@
         <v>350</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>351</v>
@@ -5899,7 +5863,7 @@
         <v>69</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>352</v>
@@ -5916,7 +5880,7 @@
         <v>353</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>354</v>
@@ -5933,7 +5897,7 @@
         <v>71</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>355</v>
@@ -5950,7 +5914,7 @@
         <v>356</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>357</v>
@@ -5967,7 +5931,7 @@
         <v>84</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>85</v>
@@ -6001,7 +5965,7 @@
         <v>89</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>360</v>
@@ -6018,7 +5982,7 @@
         <v>337</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>338</v>
@@ -6035,7 +5999,7 @@
         <v>339</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>340</v>
@@ -6052,7 +6016,7 @@
         <v>341</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>342</v>
@@ -6086,7 +6050,7 @@
         <v>92</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>363</v>
@@ -6103,7 +6067,7 @@
         <v>94</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>364</v>
@@ -6120,7 +6084,7 @@
         <v>365</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>366</v>
@@ -6137,7 +6101,7 @@
         <v>367</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>368</v>
@@ -6154,7 +6118,7 @@
         <v>319</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>320</v>
@@ -6477,7 +6441,7 @@
         <v>147</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>405</v>
@@ -6494,7 +6458,7 @@
         <v>149</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E39" s="23" t="s">
         <v>406</v>
@@ -6596,7 +6560,7 @@
         <v>164</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E45" s="23" t="s">
         <v>418</v>
@@ -6698,7 +6662,7 @@
         <v>173</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E51" s="23" t="s">
         <v>427</v>
@@ -6715,7 +6679,7 @@
         <v>428</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E52" s="23" t="s">
         <v>429</v>
@@ -6902,7 +6866,7 @@
         <v>205</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E63" s="27" t="s">
         <v>206</v>

</xml_diff>